<commit_message>
View stuff & fixes
</commit_message>
<xml_diff>
--- a/database/seeds/data/fragments.xlsx
+++ b/database/seeds/data/fragments.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21060" activeTab="1"/>
+    <workbookView xWindow="8140" yWindow="460" windowWidth="30260" windowHeight="21060"/>
   </bookViews>
   <sheets>
     <sheet name="fragments" sheetId="1" r:id="rId1"/>
     <sheet name="hidden" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">fragments!$A$2:$Z$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">fragments!$A$2:$Z$46</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="443">
   <si>
     <t>name</t>
   </si>
@@ -1354,6 +1354,9 @@
   </si>
   <si>
     <t>Nieuwstag</t>
+  </si>
+  <si>
+    <t>auth.email</t>
   </si>
 </sst>
 </file>
@@ -1733,11 +1736,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z85"/>
+  <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1818,77 +1821,80 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
+        <v>442</v>
+      </c>
+      <c r="B4" s="3">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
-        <v>220</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>199</v>
-      </c>
-      <c r="B5" s="3">
+        <v>5</v>
+      </c>
+      <c r="B5">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>201</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
       </c>
+      <c r="D6" t="s">
+        <v>201</v>
+      </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>218</v>
       </c>
       <c r="B7" s="3">
         <v>0</v>
       </c>
-      <c r="D7" t="s">
-        <v>192</v>
-      </c>
       <c r="E7" t="s">
-        <v>191</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
+        <v>190</v>
+      </c>
+      <c r="B8" s="3">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>192</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -1896,286 +1902,283 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
       <c r="E10" t="s">
-        <v>221</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>229</v>
-      </c>
-      <c r="B11" s="3">
+        <v>11</v>
+      </c>
+      <c r="B11">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>169</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>219</v>
-      </c>
-      <c r="B12">
+        <v>229</v>
+      </c>
+      <c r="B12" s="3">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>170</v>
       </c>
       <c r="E12" t="s">
-        <v>71</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>202</v>
-      </c>
-      <c r="B13" s="3">
+        <v>219</v>
+      </c>
+      <c r="B13">
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>204</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s">
-        <v>203</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B14" s="3">
         <v>0</v>
       </c>
+      <c r="D14" t="s">
+        <v>204</v>
+      </c>
       <c r="E14" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B15" s="3">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="D17" t="s">
-        <v>15</v>
+        <v>214</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>14</v>
+        <v>215</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>193</v>
-      </c>
-      <c r="B18" s="3">
+        <v>13</v>
+      </c>
+      <c r="B18">
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>195</v>
+        <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>194</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>168</v>
+        <v>193</v>
       </c>
       <c r="B19" s="3">
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>88</v>
+        <v>195</v>
       </c>
       <c r="E19" t="s">
-        <v>87</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20">
+        <v>168</v>
+      </c>
+      <c r="B20" s="3">
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>18</v>
+        <v>88</v>
       </c>
       <c r="E20" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E21" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>208</v>
-      </c>
-      <c r="B23" s="3">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>24</v>
       </c>
       <c r="E23" t="s">
-        <v>209</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B24" s="3">
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="D25" t="s">
-        <v>26</v>
+        <v>210</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E27" t="s">
-        <v>30</v>
+        <v>223</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B28">
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E28" t="s">
-        <v>224</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>226</v>
+        <v>32</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>227</v>
+        <v>33</v>
       </c>
       <c r="E29" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>226</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>35</v>
+        <v>227</v>
       </c>
       <c r="E30" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -2189,623 +2192,623 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32">
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E32" t="s">
-        <v>38</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>185</v>
-      </c>
-      <c r="B33" s="3">
+        <v>37</v>
+      </c>
+      <c r="B33">
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>187</v>
+        <v>39</v>
       </c>
       <c r="E33" t="s">
-        <v>186</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34">
+        <v>185</v>
+      </c>
+      <c r="B34" s="3">
         <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>42</v>
+        <v>187</v>
       </c>
       <c r="E34" t="s">
-        <v>41</v>
+        <v>186</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B35">
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E35" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B36">
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E36" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B37">
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="E37" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>181</v>
-      </c>
-      <c r="B38" s="3">
+        <v>49</v>
+      </c>
+      <c r="B38">
         <v>0</v>
       </c>
       <c r="D38" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E38" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B39" s="3">
         <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>180</v>
+        <v>42</v>
       </c>
       <c r="E39" t="s">
-        <v>179</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="B40" s="3">
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>33</v>
+        <v>180</v>
       </c>
       <c r="E40" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B41" s="3">
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="E41" t="s">
-        <v>10</v>
+        <v>173</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B42" s="3">
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="E42" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B43" s="3">
         <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>177</v>
+        <v>48</v>
       </c>
       <c r="E43" t="s">
-        <v>176</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>50</v>
-      </c>
-      <c r="B44">
+        <v>175</v>
+      </c>
+      <c r="B44" s="3">
         <v>0</v>
       </c>
       <c r="D44" t="s">
-        <v>52</v>
+        <v>177</v>
       </c>
       <c r="E44" t="s">
-        <v>51</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>182</v>
-      </c>
-      <c r="B45" s="3">
+        <v>50</v>
+      </c>
+      <c r="B45">
         <v>0</v>
       </c>
       <c r="D45" t="s">
-        <v>184</v>
+        <v>52</v>
       </c>
       <c r="E45" t="s">
-        <v>183</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="B46" s="3">
         <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="E46" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>61</v>
-      </c>
-      <c r="B47">
+        <v>205</v>
+      </c>
+      <c r="B47" s="3">
         <v>0</v>
       </c>
       <c r="D47" t="s">
-        <v>63</v>
+        <v>207</v>
       </c>
       <c r="E47" t="s">
-        <v>62</v>
+        <v>206</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B48">
         <v>0</v>
       </c>
       <c r="D48" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E48" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B49">
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="E49" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>67</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="D50" t="s">
+        <v>57</v>
+      </c>
+      <c r="E50" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>68</v>
       </c>
-      <c r="B50">
-        <v>0</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="D51" t="s">
         <v>70</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E51" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B51" s="3">
-        <v>0</v>
-      </c>
-      <c r="D51" t="s">
-        <v>131</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B52" s="3">
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B53" s="3">
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B54" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>140</v>
-      </c>
-      <c r="E54" t="s">
-        <v>139</v>
+        <v>134</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B55" s="3">
         <v>1</v>
       </c>
       <c r="D55" t="s">
+        <v>140</v>
+      </c>
+      <c r="E55" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B56" s="3">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
         <v>143</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E56" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>144</v>
-      </c>
-      <c r="B56" s="3">
-        <v>0</v>
-      </c>
-      <c r="D56" t="s">
-        <v>146</v>
-      </c>
-      <c r="E56" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="B57" s="3">
         <v>0</v>
       </c>
       <c r="D57" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="E57" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B58" s="3">
         <v>0</v>
       </c>
       <c r="D58" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E58" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B59" s="3">
         <v>0</v>
       </c>
       <c r="D59" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="E59" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B60" s="3">
         <v>0</v>
       </c>
       <c r="D60" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E60" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B61" s="3">
         <v>0</v>
       </c>
       <c r="D61" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E61" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="B62" s="3">
         <v>0</v>
       </c>
       <c r="D62" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="E62" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B63" s="3">
         <v>0</v>
       </c>
       <c r="D63" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E63" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>72</v>
-      </c>
-      <c r="B64">
+        <v>147</v>
+      </c>
+      <c r="B64" s="3">
         <v>0</v>
       </c>
       <c r="D64" t="s">
-        <v>74</v>
+        <v>149</v>
       </c>
       <c r="E64" t="s">
-        <v>73</v>
+        <v>148</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B65">
         <v>0</v>
       </c>
       <c r="D65" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="E65" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B66">
         <v>0</v>
       </c>
       <c r="D66" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="E66" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B67">
         <v>0</v>
       </c>
       <c r="D67" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E67" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B68">
         <v>0</v>
       </c>
       <c r="D68" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E68" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B69">
         <v>0</v>
       </c>
       <c r="D69" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="E69" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B70">
         <v>0</v>
       </c>
       <c r="D70" t="s">
-        <v>88</v>
+        <v>15</v>
       </c>
       <c r="E70" t="s">
-        <v>87</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B71">
         <v>0</v>
       </c>
       <c r="D71" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="E71" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B72">
         <v>0</v>
       </c>
       <c r="D72" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="E72" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>90</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+      <c r="D73" t="s">
+        <v>92</v>
+      </c>
+      <c r="E73" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>93</v>
       </c>
-      <c r="B73">
-        <v>0</v>
-      </c>
-      <c r="D73" t="s">
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="D74" t="s">
         <v>95</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E74" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B74" s="3">
-        <v>0</v>
-      </c>
-      <c r="D74" t="s">
-        <v>104</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B75" s="3">
         <v>0</v>
       </c>
       <c r="D75" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B76" s="3">
         <v>0</v>
@@ -2814,132 +2817,146 @@
         <v>107</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B77" s="3">
         <v>0</v>
       </c>
       <c r="D77" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="B78" s="3">
         <v>0</v>
       </c>
       <c r="D78" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="B79" s="3">
         <v>0</v>
       </c>
       <c r="D79" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B80" s="3">
         <v>0</v>
       </c>
       <c r="D80" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="B81" s="3">
         <v>0</v>
       </c>
       <c r="D81" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B82" s="3">
         <v>0</v>
       </c>
       <c r="D82" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="B83" s="3">
         <v>0</v>
       </c>
       <c r="D83" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="B84" s="3">
         <v>0</v>
       </c>
       <c r="D84" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B85" s="3">
+        <v>0</v>
+      </c>
+      <c r="D85" t="s">
+        <v>122</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B85" s="3">
-        <v>0</v>
-      </c>
-      <c r="D85" t="s">
+      <c r="B86" s="3">
+        <v>0</v>
+      </c>
+      <c r="D86" t="s">
         <v>125</v>
       </c>
-      <c r="E85" s="2" t="s">
+      <c r="E86" s="2" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2957,7 +2974,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>

<commit_message>
adjust front views titles & metadescription
</commit_message>
<xml_diff>
--- a/database/seeds/data/fragments.xlsx
+++ b/database/seeds/data/fragments.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26606"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27011"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiandedeyne/Sites/blender/database/seeds/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/willem/Sites/blender/database/seeds/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17620" activeTab="1"/>
+    <workbookView xWindow="20540" yWindow="3380" windowWidth="28800" windowHeight="17620"/>
   </bookViews>
   <sheets>
     <sheet name="fragments" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,9 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="479">
   <si>
     <t>name</t>
   </si>
@@ -1447,6 +1450,21 @@
   </si>
   <si>
     <t>Uitloggen</t>
+  </si>
+  <si>
+    <t>home.title</t>
+  </si>
+  <si>
+    <t>home.metaDescription</t>
+  </si>
+  <si>
+    <t>Home titel</t>
+  </si>
+  <si>
+    <t>Home titre</t>
+  </si>
+  <si>
+    <t>Home metadescription</t>
   </si>
 </sst>
 </file>
@@ -1802,11 +1820,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z16"/>
+  <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2067,6 +2085,34 @@
         <v>48</v>
       </c>
     </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>474</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>476</v>
+      </c>
+      <c r="E17" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>475</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>478</v>
+      </c>
+      <c r="E18" t="s">
+        <v>478</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
@@ -2081,7 +2127,7 @@
   </sheetPr>
   <dimension ref="A1:Z221"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>

</xml_diff>

<commit_message>
Refactored mailer service & cleaned up fragments
</commit_message>
<xml_diff>
--- a/database/seeds/data/fragments.xlsx
+++ b/database/seeds/data/fragments.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26606"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/willem/Sites/blender/database/seeds/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiandedeyne/Sites/blender/database/seeds/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20540" yWindow="3380" windowWidth="28800" windowHeight="17620"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="fragments" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,6 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -28,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="463">
   <si>
     <t>name</t>
   </si>
@@ -198,15 +195,6 @@
     <t>Stad</t>
   </si>
   <si>
-    <t>auth.correctFormErrors</t>
-  </si>
-  <si>
-    <t>Corrigeer de fouten hieronder.</t>
-  </si>
-  <si>
-    <t>Corrigez les erreurs plus bas.</t>
-  </si>
-  <si>
     <t>auth.country</t>
   </si>
   <si>
@@ -249,9 +237,6 @@
     <t>Naam</t>
   </si>
   <si>
-    <t>auth.linkValidUntil</t>
-  </si>
-  <si>
     <t>Ce lien est valable jusqu'au</t>
   </si>
   <si>
@@ -273,12 +258,6 @@
     <t>Login</t>
   </si>
   <si>
-    <t>auth.login.welcome</t>
-  </si>
-  <si>
-    <t>Welkom bij Blender. Gelieve hier in te loggen.</t>
-  </si>
-  <si>
     <t>auth.logout.title</t>
   </si>
   <si>
@@ -303,15 +282,6 @@
     <t>Votre compte n'est pas encore actif.</t>
   </si>
   <si>
-    <t>auth.oldUser.intro</t>
-  </si>
-  <si>
-    <t>auth.oldUser.outro</t>
-  </si>
-  <si>
-    <t>auth.oldUser.resetButton</t>
-  </si>
-  <si>
     <t>auth.password</t>
   </si>
   <si>
@@ -336,15 +306,9 @@
     <t>Che(è)r(e)</t>
   </si>
   <si>
-    <t>auth.passwordMail.intro</t>
-  </si>
-  <si>
     <t>Je hebt toegang gekregen tot</t>
   </si>
   <si>
-    <t>Vous avez êtes admis l'accès à</t>
-  </si>
-  <si>
     <t>auth.passwordMail.linkValidUntil</t>
   </si>
   <si>
@@ -360,18 +324,12 @@
     <t>auth.passwordMail.oldUser.intro</t>
   </si>
   <si>
-    <t>We ontvingen je vraag om je Blender wachtwoord te wijzigen op</t>
-  </si>
-  <si>
     <t>Nous avons reçu une demande de changer votre mot de passe</t>
   </si>
   <si>
     <t>auth.passwordMail.oldUser.outro</t>
   </si>
   <si>
-    <t>Was het een foutieve aanvraag? Negeer dan deze e-mail, je oude paswoord blijft gewoon werken.</t>
-  </si>
-  <si>
     <t>Dans le cas où vous avez fait la demande noot une réinitialisation de mot de passe , ignorez ce e-mail.</t>
   </si>
   <si>
@@ -384,9 +342,6 @@
     <t>Changer le mot de passe</t>
   </si>
   <si>
-    <t>auth.passwordMail.resetButton</t>
-  </si>
-  <si>
     <t>Wachtwoord instellen</t>
   </si>
   <si>
@@ -411,9 +366,6 @@
     <t>Créez votre profil</t>
   </si>
   <si>
-    <t>auth.register.title</t>
-  </si>
-  <si>
     <t>auth.register.toLogin</t>
   </si>
   <si>
@@ -1452,19 +1404,16 @@
     <t>Uitloggen</t>
   </si>
   <si>
-    <t>home.title</t>
-  </si>
-  <si>
-    <t>home.metaDescription</t>
-  </si>
-  <si>
-    <t>Home titel</t>
-  </si>
-  <si>
-    <t>Home titre</t>
-  </si>
-  <si>
-    <t>Home metadescription</t>
+    <t>auth.titleRegister</t>
+  </si>
+  <si>
+    <t>We ontvingen je vraag om je wachtwoord te wijzigen op</t>
+  </si>
+  <si>
+    <t>Was het een foutieve aanvraag? Negeer dan deze e-mail, je oude wachtwoord blijft gewoon werken.</t>
+  </si>
+  <si>
+    <t>back.auth.titleChangePassword</t>
   </si>
 </sst>
 </file>
@@ -1820,11 +1769,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z18"/>
+  <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2085,34 +2034,6 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>474</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="D17" t="s">
-        <v>476</v>
-      </c>
-      <c r="E17" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>475</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="D18" t="s">
-        <v>478</v>
-      </c>
-      <c r="E18" t="s">
-        <v>478</v>
-      </c>
-    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
@@ -2125,11 +2046,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z221"/>
+  <dimension ref="A1:Z214"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2137,7 +2058,7 @@
     <col min="1" max="1" width="53" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="187.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80" customWidth="1"/>
     <col min="5" max="5" width="133.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="26" width="1.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2226,55 +2147,55 @@
       <c r="D5" t="s">
         <v>57</v>
       </c>
-      <c r="E5" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" t="s">
         <v>64</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
@@ -2301,9 +2222,6 @@
       <c r="D11" t="s">
         <v>69</v>
       </c>
-      <c r="E11" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -2315,391 +2233,421 @@
       <c r="D12" t="s">
         <v>72</v>
       </c>
+      <c r="E12" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
+      <c r="D13" t="s">
+        <v>75</v>
+      </c>
       <c r="E13" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>457</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>76</v>
-      </c>
-      <c r="E14" t="s">
-        <v>77</v>
+        <v>458</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
         <v>78</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="D15" t="s">
-        <v>79</v>
-      </c>
       <c r="E15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" t="s">
         <v>81</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="D16" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>472</v>
+        <v>82</v>
       </c>
       <c r="B17">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>473</v>
+        <v>83</v>
+      </c>
+      <c r="E17" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>84</v>
-      </c>
-      <c r="E18" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E19" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="E20" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
         <v>91</v>
       </c>
-      <c r="B21">
-        <v>0</v>
+      <c r="E21" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B22">
         <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
         <v>93</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B25">
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>96</v>
+        <v>460</v>
       </c>
       <c r="E25" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>38</v>
+        <v>461</v>
       </c>
       <c r="E26" t="s">
-        <v>39</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E27" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B28">
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>103</v>
-      </c>
-      <c r="E28" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>106</v>
-      </c>
-      <c r="E29" t="s">
-        <v>74</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B30">
         <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>111</v>
+      </c>
+      <c r="E30" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B31">
         <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>114</v>
+      </c>
+      <c r="E31" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B32">
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E32" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="E33" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="B34">
         <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="E34" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B35">
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="E35" t="s">
-        <v>36</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B36">
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>121</v>
+        <v>129</v>
+      </c>
+      <c r="E36" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="B37">
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>123</v>
+        <v>114</v>
+      </c>
+      <c r="E37" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>132</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="D38" t="s">
+        <v>123</v>
+      </c>
+      <c r="E38" t="s">
         <v>124</v>
-      </c>
-      <c r="B38">
-        <v>0</v>
-      </c>
-      <c r="D38" t="s">
-        <v>125</v>
-      </c>
-      <c r="E38" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B39">
         <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="E39" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="B40">
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="E40" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="B41">
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>132</v>
-      </c>
-      <c r="E41" t="s">
-        <v>133</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="B42">
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>135</v>
+        <v>76</v>
       </c>
       <c r="E42" t="s">
-        <v>136</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>137</v>
+        <v>459</v>
       </c>
       <c r="B43">
         <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>138</v>
+        <v>111</v>
       </c>
       <c r="E43" t="s">
-        <v>139</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -2710,38 +2658,38 @@
         <v>0</v>
       </c>
       <c r="D44" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="E44" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>141</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="D45" t="s">
+        <v>142</v>
+      </c>
+      <c r="E45" t="s">
         <v>143</v>
-      </c>
-      <c r="B45">
-        <v>0</v>
-      </c>
-      <c r="D45" t="s">
-        <v>144</v>
-      </c>
-      <c r="E45" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="D46" t="s">
+        <v>145</v>
+      </c>
+      <c r="E46" t="s">
         <v>146</v>
-      </c>
-      <c r="B46">
-        <v>0</v>
-      </c>
-      <c r="D46" t="s">
-        <v>129</v>
-      </c>
-      <c r="E46" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -2752,136 +2700,115 @@
         <v>0</v>
       </c>
       <c r="D47" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="E47" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B48">
         <v>0</v>
       </c>
       <c r="D48" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E48" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B49">
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>44</v>
-      </c>
-      <c r="E49" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B50">
         <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B51">
         <v>0</v>
       </c>
       <c r="D51" t="s">
-        <v>80</v>
-      </c>
-      <c r="E51" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B52">
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>144</v>
-      </c>
-      <c r="E52" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="B53">
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>157</v>
-      </c>
-      <c r="E53" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B54">
         <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>160</v>
-      </c>
-      <c r="E54" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B55">
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>163</v>
-      </c>
-      <c r="E55" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B56">
         <v>0</v>
       </c>
       <c r="D56" t="s">
-        <v>166</v>
-      </c>
-      <c r="E56" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>168</v>
       </c>
@@ -2892,7 +2819,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>170</v>
       </c>
@@ -2903,7 +2830,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>172</v>
       </c>
@@ -2914,7 +2841,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>174</v>
       </c>
@@ -2925,7 +2852,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>176</v>
       </c>
@@ -2936,7 +2863,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>178</v>
       </c>
@@ -2944,21 +2871,21 @@
         <v>0</v>
       </c>
       <c r="D62" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B63">
         <v>0</v>
       </c>
       <c r="D63" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>181</v>
       </c>
@@ -2966,1817 +2893,1740 @@
         <v>0</v>
       </c>
       <c r="D64" t="s">
-        <v>182</v>
+        <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B65">
         <v>0</v>
       </c>
       <c r="D65" t="s">
-        <v>184</v>
+        <v>75</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B66">
         <v>0</v>
       </c>
       <c r="D66" t="s">
-        <v>186</v>
+        <v>35</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>187</v>
+        <v>440</v>
       </c>
       <c r="B67">
         <v>0</v>
       </c>
       <c r="D67" t="s">
-        <v>188</v>
+        <v>38</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>189</v>
+        <v>439</v>
       </c>
       <c r="B68">
         <v>0</v>
       </c>
       <c r="D68" t="s">
-        <v>190</v>
+        <v>117</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B69">
         <v>0</v>
       </c>
       <c r="D69" t="s">
-        <v>192</v>
+        <v>123</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="B70">
         <v>0</v>
       </c>
       <c r="D70" t="s">
-        <v>194</v>
+        <v>126</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B71">
         <v>0</v>
       </c>
       <c r="D71" t="s">
-        <v>24</v>
+        <v>129</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>196</v>
+        <v>462</v>
       </c>
       <c r="B72">
         <v>0</v>
       </c>
       <c r="D72" t="s">
-        <v>66</v>
+        <v>105</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>197</v>
+        <v>442</v>
       </c>
       <c r="B73">
         <v>0</v>
       </c>
       <c r="D73" t="s">
-        <v>79</v>
+        <v>443</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>198</v>
-      </c>
-      <c r="B74">
-        <v>0</v>
-      </c>
-      <c r="D74" t="s">
-        <v>35</v>
+      <c r="A74" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="B74" s="3">
+        <v>0</v>
+      </c>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>455</v>
-      </c>
-      <c r="B75">
-        <v>0</v>
-      </c>
-      <c r="D75" t="s">
-        <v>38</v>
+      <c r="A75" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="B75" s="3">
+        <v>0</v>
+      </c>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>454</v>
+        <v>187</v>
       </c>
       <c r="B76">
         <v>0</v>
       </c>
       <c r="D76" t="s">
-        <v>132</v>
+        <v>188</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="B77">
         <v>0</v>
       </c>
       <c r="D77" t="s">
-        <v>138</v>
+        <v>190</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B78">
         <v>0</v>
       </c>
       <c r="D78" t="s">
-        <v>141</v>
+        <v>26</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="B79">
         <v>0</v>
       </c>
       <c r="D79" t="s">
-        <v>144</v>
+        <v>193</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>457</v>
+        <v>194</v>
       </c>
       <c r="B80">
         <v>0</v>
       </c>
       <c r="D80" t="s">
-        <v>458</v>
+        <v>195</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="B81" s="3">
-        <v>0</v>
-      </c>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3" t="s">
-        <v>144</v>
+      <c r="A81" t="s">
+        <v>196</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="D81" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="3" t="s">
-        <v>447</v>
-      </c>
-      <c r="B82" s="3">
-        <v>0</v>
-      </c>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3" t="s">
-        <v>448</v>
+      <c r="A82" t="s">
+        <v>197</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="D82" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B83">
         <v>0</v>
       </c>
       <c r="D83" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B84">
         <v>0</v>
       </c>
       <c r="D84" t="s">
-        <v>205</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B85">
         <v>0</v>
       </c>
       <c r="D85" t="s">
-        <v>26</v>
+        <v>203</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B86">
         <v>0</v>
       </c>
       <c r="D86" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B87">
         <v>0</v>
       </c>
       <c r="D87" t="s">
-        <v>210</v>
+        <v>35</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B88">
         <v>0</v>
       </c>
       <c r="D88" t="s">
-        <v>29</v>
+        <v>208</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B89">
         <v>0</v>
       </c>
       <c r="D89" t="s">
-        <v>213</v>
+        <v>38</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B90">
         <v>0</v>
       </c>
       <c r="D90" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B91">
         <v>0</v>
       </c>
       <c r="D91" t="s">
-        <v>72</v>
+        <v>213</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B92">
         <v>0</v>
       </c>
       <c r="D92" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B93">
         <v>0</v>
       </c>
       <c r="D93" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>221</v>
+        <v>444</v>
       </c>
       <c r="B94">
         <v>0</v>
       </c>
       <c r="D94" t="s">
-        <v>35</v>
+        <v>449</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B95">
         <v>0</v>
       </c>
       <c r="D95" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B96">
         <v>0</v>
       </c>
       <c r="D96" t="s">
-        <v>38</v>
+        <v>221</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B97">
         <v>0</v>
       </c>
       <c r="D97" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B98">
         <v>0</v>
       </c>
       <c r="D98" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B99">
         <v>0</v>
       </c>
       <c r="D99" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B100">
         <v>0</v>
       </c>
       <c r="D100" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>459</v>
+        <v>230</v>
       </c>
       <c r="B101">
         <v>0</v>
       </c>
       <c r="D101" t="s">
-        <v>464</v>
+        <v>231</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B102">
         <v>0</v>
       </c>
       <c r="D102" t="s">
-        <v>234</v>
+        <v>441</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B103">
         <v>0</v>
       </c>
       <c r="D103" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B104">
         <v>0</v>
       </c>
       <c r="D104" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>239</v>
+        <v>446</v>
       </c>
       <c r="B105">
         <v>0</v>
       </c>
       <c r="D105" t="s">
-        <v>240</v>
+        <v>451</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B106">
         <v>0</v>
       </c>
       <c r="D106" t="s">
-        <v>242</v>
+        <v>69</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B107">
         <v>0</v>
       </c>
       <c r="D107" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B108">
         <v>0</v>
       </c>
       <c r="D108" t="s">
-        <v>246</v>
+        <v>177</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="B109">
         <v>0</v>
       </c>
       <c r="D109" t="s">
-        <v>456</v>
+        <v>242</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B110">
         <v>0</v>
       </c>
       <c r="D110" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B111">
         <v>0</v>
       </c>
       <c r="D111" t="s">
-        <v>251</v>
+        <v>26</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>461</v>
+        <v>246</v>
       </c>
       <c r="B112">
         <v>0</v>
       </c>
       <c r="D112" t="s">
-        <v>466</v>
+        <v>195</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B113">
         <v>0</v>
       </c>
       <c r="D113" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B114">
         <v>0</v>
       </c>
       <c r="D114" t="s">
-        <v>254</v>
+        <v>198</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="B115">
         <v>0</v>
       </c>
       <c r="D115" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B116">
         <v>0</v>
       </c>
       <c r="D116" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B117">
         <v>0</v>
       </c>
       <c r="D117" t="s">
-        <v>259</v>
+        <v>69</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="B118">
         <v>0</v>
       </c>
       <c r="D118" t="s">
-        <v>26</v>
+        <v>203</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="B119">
         <v>0</v>
       </c>
       <c r="D119" t="s">
-        <v>210</v>
+        <v>255</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B120">
         <v>0</v>
       </c>
       <c r="D120" t="s">
-        <v>29</v>
+        <v>257</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B121">
         <v>0</v>
       </c>
       <c r="D121" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="B122">
         <v>0</v>
       </c>
       <c r="D122" t="s">
-        <v>215</v>
+        <v>260</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B123">
         <v>0</v>
       </c>
       <c r="D123" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B124">
         <v>0</v>
       </c>
       <c r="D124" t="s">
-        <v>72</v>
+        <v>264</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B125">
         <v>0</v>
       </c>
       <c r="D125" t="s">
-        <v>218</v>
+        <v>266</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B126">
         <v>0</v>
       </c>
       <c r="D126" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B127">
         <v>0</v>
       </c>
       <c r="D127" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B128">
         <v>0</v>
       </c>
       <c r="D128" t="s">
-        <v>226</v>
+        <v>272</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
+        <v>273</v>
+      </c>
+      <c r="B129">
+        <v>0</v>
+      </c>
+      <c r="D129" t="s">
         <v>274</v>
-      </c>
-      <c r="B129">
-        <v>0</v>
-      </c>
-      <c r="D129" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
+        <v>275</v>
+      </c>
+      <c r="B130">
+        <v>0</v>
+      </c>
+      <c r="D130" t="s">
         <v>276</v>
-      </c>
-      <c r="B130">
-        <v>0</v>
-      </c>
-      <c r="D130" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>278</v>
+        <v>445</v>
       </c>
       <c r="B131">
         <v>0</v>
       </c>
       <c r="D131" t="s">
-        <v>279</v>
+        <v>450</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B132">
         <v>0</v>
       </c>
       <c r="D132" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B133">
         <v>0</v>
       </c>
       <c r="D133" t="s">
-        <v>283</v>
+        <v>69</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>284</v>
+        <v>453</v>
       </c>
       <c r="B134">
         <v>0</v>
       </c>
       <c r="D134" t="s">
-        <v>285</v>
+        <v>456</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>286</v>
+        <v>454</v>
       </c>
       <c r="B135">
         <v>0</v>
       </c>
       <c r="D135" t="s">
-        <v>287</v>
+        <v>236</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>288</v>
+        <v>452</v>
       </c>
       <c r="B136">
         <v>0</v>
       </c>
       <c r="D136" t="s">
-        <v>289</v>
+        <v>455</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="B137">
         <v>0</v>
       </c>
       <c r="D137" t="s">
-        <v>291</v>
+        <v>158</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>460</v>
+        <v>281</v>
       </c>
       <c r="B138">
         <v>0</v>
       </c>
       <c r="D138" t="s">
-        <v>465</v>
+        <v>160</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="B139">
         <v>0</v>
       </c>
       <c r="D139" t="s">
-        <v>293</v>
+        <v>69</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="B140">
         <v>0</v>
       </c>
       <c r="D140" t="s">
-        <v>72</v>
+        <v>284</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>468</v>
+        <v>285</v>
       </c>
       <c r="B141">
         <v>0</v>
       </c>
       <c r="D141" t="s">
-        <v>471</v>
+        <v>286</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>469</v>
+        <v>287</v>
       </c>
       <c r="B142">
         <v>0</v>
       </c>
       <c r="D142" t="s">
-        <v>251</v>
+        <v>175</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>467</v>
+        <v>288</v>
       </c>
       <c r="B143">
         <v>0</v>
       </c>
       <c r="D143" t="s">
-        <v>470</v>
+        <v>167</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="B144">
         <v>0</v>
       </c>
       <c r="D144" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B145">
         <v>0</v>
       </c>
       <c r="D145" t="s">
-        <v>175</v>
+        <v>291</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="B146">
         <v>0</v>
       </c>
       <c r="D146" t="s">
-        <v>72</v>
+        <v>293</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B147">
         <v>0</v>
       </c>
       <c r="D147" t="s">
-        <v>299</v>
+        <v>175</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="B148">
         <v>0</v>
       </c>
       <c r="D148" t="s">
-        <v>301</v>
+        <v>177</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B149">
         <v>0</v>
       </c>
       <c r="D149" t="s">
-        <v>190</v>
+        <v>297</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B150">
         <v>0</v>
       </c>
       <c r="D150" t="s">
-        <v>182</v>
+        <v>299</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B151">
         <v>0</v>
       </c>
       <c r="D151" t="s">
-        <v>184</v>
+        <v>24</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B152">
         <v>0</v>
       </c>
       <c r="D152" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B153">
         <v>0</v>
       </c>
       <c r="D153" t="s">
-        <v>308</v>
+        <v>160</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B154">
         <v>0</v>
       </c>
       <c r="D154" t="s">
-        <v>190</v>
+        <v>69</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="B155">
         <v>0</v>
       </c>
       <c r="D155" t="s">
-        <v>192</v>
+        <v>306</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B156">
         <v>0</v>
       </c>
       <c r="D156" t="s">
-        <v>312</v>
+        <v>167</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B157">
         <v>0</v>
       </c>
       <c r="D157" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="B158">
         <v>0</v>
       </c>
       <c r="D158" t="s">
-        <v>24</v>
+        <v>311</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B159">
         <v>0</v>
       </c>
       <c r="D159" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B160">
         <v>0</v>
       </c>
       <c r="D160" t="s">
-        <v>175</v>
+        <v>315</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B161">
         <v>0</v>
       </c>
       <c r="D161" t="s">
-        <v>72</v>
+        <v>317</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B162">
         <v>0</v>
       </c>
       <c r="D162" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B163">
         <v>0</v>
       </c>
       <c r="D163" t="s">
-        <v>182</v>
+        <v>321</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
+        <v>322</v>
+      </c>
+      <c r="B164">
+        <v>0</v>
+      </c>
+      <c r="D164" t="s">
         <v>323</v>
-      </c>
-      <c r="B164">
-        <v>0</v>
-      </c>
-      <c r="D164" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
+        <v>324</v>
+      </c>
+      <c r="B165">
+        <v>0</v>
+      </c>
+      <c r="D165" t="s">
         <v>325</v>
-      </c>
-      <c r="B165">
-        <v>0</v>
-      </c>
-      <c r="D165" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
+        <v>326</v>
+      </c>
+      <c r="B166">
+        <v>0</v>
+      </c>
+      <c r="D166" t="s">
         <v>327</v>
-      </c>
-      <c r="B166">
-        <v>0</v>
-      </c>
-      <c r="D166" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
+        <v>328</v>
+      </c>
+      <c r="B167">
+        <v>0</v>
+      </c>
+      <c r="D167" t="s">
         <v>329</v>
-      </c>
-      <c r="B167">
-        <v>0</v>
-      </c>
-      <c r="D167" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
+        <v>330</v>
+      </c>
+      <c r="B168">
+        <v>0</v>
+      </c>
+      <c r="D168" t="s">
         <v>331</v>
-      </c>
-      <c r="B168">
-        <v>0</v>
-      </c>
-      <c r="D168" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
+        <v>332</v>
+      </c>
+      <c r="B169">
+        <v>0</v>
+      </c>
+      <c r="D169" t="s">
         <v>333</v>
-      </c>
-      <c r="B169">
-        <v>0</v>
-      </c>
-      <c r="D169" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
+        <v>334</v>
+      </c>
+      <c r="B170">
+        <v>0</v>
+      </c>
+      <c r="D170" t="s">
         <v>335</v>
-      </c>
-      <c r="B170">
-        <v>0</v>
-      </c>
-      <c r="D170" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
+        <v>336</v>
+      </c>
+      <c r="B171">
+        <v>0</v>
+      </c>
+      <c r="D171" t="s">
         <v>337</v>
-      </c>
-      <c r="B171">
-        <v>0</v>
-      </c>
-      <c r="D171" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
+        <v>338</v>
+      </c>
+      <c r="B172">
+        <v>0</v>
+      </c>
+      <c r="D172" t="s">
         <v>339</v>
-      </c>
-      <c r="B172">
-        <v>0</v>
-      </c>
-      <c r="D172" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
+        <v>340</v>
+      </c>
+      <c r="B173">
+        <v>0</v>
+      </c>
+      <c r="D173" t="s">
         <v>341</v>
-      </c>
-      <c r="B173">
-        <v>0</v>
-      </c>
-      <c r="D173" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
+        <v>342</v>
+      </c>
+      <c r="B174">
+        <v>0</v>
+      </c>
+      <c r="D174" t="s">
         <v>343</v>
-      </c>
-      <c r="B174">
-        <v>0</v>
-      </c>
-      <c r="D174" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
+        <v>344</v>
+      </c>
+      <c r="B175">
+        <v>0</v>
+      </c>
+      <c r="D175" t="s">
         <v>345</v>
-      </c>
-      <c r="B175">
-        <v>0</v>
-      </c>
-      <c r="D175" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
+        <v>346</v>
+      </c>
+      <c r="B176">
+        <v>0</v>
+      </c>
+      <c r="D176" t="s">
         <v>347</v>
       </c>
-      <c r="B176">
-        <v>0</v>
-      </c>
-      <c r="D176" t="s">
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A177" t="s">
+      <c r="B177">
+        <v>0</v>
+      </c>
+      <c r="D177" t="s">
         <v>349</v>
       </c>
-      <c r="B177">
-        <v>0</v>
-      </c>
-      <c r="D177" t="s">
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A178" t="s">
+      <c r="B178">
+        <v>0</v>
+      </c>
+      <c r="D178" t="s">
         <v>351</v>
       </c>
-      <c r="B178">
-        <v>0</v>
-      </c>
-      <c r="D178" t="s">
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A179" t="s">
+      <c r="B179">
+        <v>0</v>
+      </c>
+      <c r="D179" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
         <v>353</v>
       </c>
-      <c r="B179">
-        <v>0</v>
-      </c>
-      <c r="D179" t="s">
+      <c r="B180">
+        <v>0</v>
+      </c>
+      <c r="D180" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A180" t="s">
+      <c r="B181">
+        <v>0</v>
+      </c>
+      <c r="D181" t="s">
         <v>355</v>
       </c>
-      <c r="B180">
-        <v>0</v>
-      </c>
-      <c r="D180" t="s">
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A181" t="s">
+      <c r="B182">
+        <v>0</v>
+      </c>
+      <c r="D182" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
         <v>357</v>
       </c>
-      <c r="B181">
-        <v>0</v>
-      </c>
-      <c r="D181" t="s">
+      <c r="B183">
+        <v>0</v>
+      </c>
+      <c r="D183" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A182" t="s">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
         <v>359</v>
       </c>
-      <c r="B182">
-        <v>0</v>
-      </c>
-      <c r="D182" t="s">
+      <c r="B184">
+        <v>0</v>
+      </c>
+      <c r="D184" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A183" t="s">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
         <v>361</v>
       </c>
-      <c r="B183">
-        <v>0</v>
-      </c>
-      <c r="D183" t="s">
+      <c r="B185">
+        <v>0</v>
+      </c>
+      <c r="D185" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A184" t="s">
+      <c r="B186">
+        <v>0</v>
+      </c>
+      <c r="D186" t="s">
         <v>363</v>
       </c>
-      <c r="B184">
-        <v>0</v>
-      </c>
-      <c r="D184" t="s">
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A185" t="s">
+      <c r="B187">
+        <v>0</v>
+      </c>
+      <c r="D187" t="s">
         <v>365</v>
       </c>
-      <c r="B185">
-        <v>0</v>
-      </c>
-      <c r="D185" t="s">
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A186" t="s">
+      <c r="B188">
+        <v>0</v>
+      </c>
+      <c r="D188" t="s">
         <v>367</v>
       </c>
-      <c r="B186">
-        <v>0</v>
-      </c>
-      <c r="D186" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A187" t="s">
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>447</v>
+      </c>
+      <c r="B189">
+        <v>0</v>
+      </c>
+      <c r="D189" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>448</v>
+      </c>
+      <c r="B190">
+        <v>0</v>
+      </c>
+      <c r="D190" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
         <v>368</v>
       </c>
-      <c r="B187">
-        <v>0</v>
-      </c>
-      <c r="D187" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A188" t="s">
+      <c r="B191">
+        <v>1</v>
+      </c>
+      <c r="D191" t="s">
         <v>369</v>
       </c>
-      <c r="B188">
-        <v>0</v>
-      </c>
-      <c r="D188" t="s">
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A189" t="s">
+      <c r="B192">
+        <v>0</v>
+      </c>
+      <c r="D192" t="s">
         <v>371</v>
       </c>
-      <c r="B189">
-        <v>0</v>
-      </c>
-      <c r="D189" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A190" t="s">
+      <c r="E192" t="s">
         <v>372</v>
-      </c>
-      <c r="B190">
-        <v>0</v>
-      </c>
-      <c r="D190" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A191" t="s">
-        <v>374</v>
-      </c>
-      <c r="B191">
-        <v>0</v>
-      </c>
-      <c r="D191" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A192" t="s">
-        <v>376</v>
-      </c>
-      <c r="B192">
-        <v>0</v>
-      </c>
-      <c r="D192" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B193">
         <v>0</v>
       </c>
       <c r="D193" t="s">
-        <v>378</v>
+        <v>374</v>
+      </c>
+      <c r="E193" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B194">
         <v>0</v>
       </c>
       <c r="D194" t="s">
-        <v>380</v>
+        <v>377</v>
+      </c>
+      <c r="E194" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
+        <v>379</v>
+      </c>
+      <c r="B195">
+        <v>0</v>
+      </c>
+      <c r="D195" t="s">
+        <v>380</v>
+      </c>
+      <c r="E195" t="s">
         <v>381</v>
-      </c>
-      <c r="B195">
-        <v>0</v>
-      </c>
-      <c r="D195" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>462</v>
+        <v>382</v>
       </c>
       <c r="B196">
         <v>0</v>
       </c>
       <c r="D196" t="s">
-        <v>210</v>
+        <v>383</v>
+      </c>
+      <c r="E196" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>463</v>
+        <v>385</v>
       </c>
       <c r="B197">
         <v>0</v>
       </c>
       <c r="D197" t="s">
-        <v>218</v>
+        <v>386</v>
+      </c>
+      <c r="E197" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
       <c r="B198">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D198" t="s">
-        <v>384</v>
+        <v>435</v>
+      </c>
+      <c r="E198" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="B199">
         <v>0</v>
       </c>
       <c r="D199" t="s">
-        <v>386</v>
+        <v>438</v>
       </c>
       <c r="E199" t="s">
-        <v>387</v>
+        <v>436</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B200">
         <v>0</v>
       </c>
       <c r="D200" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="E200" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B201">
         <v>0</v>
       </c>
       <c r="D201" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="E201" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="B202">
         <v>0</v>
       </c>
       <c r="D202" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="E202" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A203" t="s">
-        <v>397</v>
-      </c>
-      <c r="B203">
-        <v>0</v>
-      </c>
-      <c r="D203" t="s">
-        <v>398</v>
+      <c r="A203" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="B203" s="2">
+        <v>0</v>
+      </c>
+      <c r="C203" s="2"/>
+      <c r="D203" s="2" t="s">
+        <v>400</v>
       </c>
       <c r="E203" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A204" t="s">
-        <v>400</v>
-      </c>
-      <c r="B204">
-        <v>0</v>
-      </c>
-      <c r="D204" t="s">
-        <v>401</v>
+      <c r="A204" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="B204" s="2">
+        <v>0</v>
+      </c>
+      <c r="C204" s="2"/>
+      <c r="D204" s="2" t="s">
+        <v>403</v>
       </c>
       <c r="E204" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
+        <v>405</v>
+      </c>
+      <c r="B205">
+        <v>0</v>
+      </c>
+      <c r="D205" t="s">
         <v>403</v>
       </c>
-      <c r="B205">
-        <v>0</v>
-      </c>
-      <c r="D205" t="s">
-        <v>450</v>
-      </c>
       <c r="E205" t="s">
-        <v>452</v>
+        <v>406</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A206" t="s">
-        <v>404</v>
-      </c>
-      <c r="B206">
-        <v>0</v>
-      </c>
-      <c r="D206" t="s">
-        <v>453</v>
+      <c r="A206" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="B206" s="3">
+        <v>0</v>
+      </c>
+      <c r="C206" s="3"/>
+      <c r="D206" s="3" t="s">
+        <v>408</v>
       </c>
       <c r="E206" t="s">
-        <v>451</v>
+        <v>409</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A207" t="s">
-        <v>405</v>
-      </c>
-      <c r="B207">
-        <v>0</v>
-      </c>
-      <c r="D207" t="s">
-        <v>406</v>
+      <c r="A207" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="B207" s="3">
+        <v>0</v>
+      </c>
+      <c r="C207" s="3"/>
+      <c r="D207" s="3" t="s">
+        <v>411</v>
       </c>
       <c r="E207" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="B208">
         <v>0</v>
       </c>
       <c r="D208" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="E208" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="B209">
         <v>0</v>
       </c>
       <c r="D209" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="E209" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A210" s="2" t="s">
+      <c r="A210" t="s">
+        <v>419</v>
+      </c>
+      <c r="B210">
+        <v>0</v>
+      </c>
+      <c r="D210" t="s">
+        <v>420</v>
+      </c>
+      <c r="E210" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A211" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="B211" s="3">
+        <v>0</v>
+      </c>
+      <c r="C211" s="3"/>
+      <c r="D211" s="3" t="s">
         <v>414</v>
       </c>
-      <c r="B210" s="2">
-        <v>0</v>
-      </c>
-      <c r="C210" s="2"/>
-      <c r="D210" s="2" t="s">
+      <c r="E211" t="s">
         <v>415</v>
       </c>
-      <c r="E210" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A211" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="B211" s="2">
-        <v>0</v>
-      </c>
-      <c r="C211" s="2"/>
-      <c r="D211" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="E211" t="s">
-        <v>419</v>
-      </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A212" t="s">
-        <v>420</v>
-      </c>
-      <c r="B212">
-        <v>0</v>
-      </c>
-      <c r="D212" t="s">
-        <v>418</v>
+      <c r="A212" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="B212" s="3">
+        <v>0</v>
+      </c>
+      <c r="C212" s="3"/>
+      <c r="D212" s="3" t="s">
+        <v>424</v>
       </c>
       <c r="E212" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A213" s="3" t="s">
-        <v>422</v>
-      </c>
-      <c r="B213" s="3">
-        <v>0</v>
-      </c>
-      <c r="C213" s="3"/>
-      <c r="D213" s="3" t="s">
-        <v>423</v>
+      <c r="A213" t="s">
+        <v>426</v>
+      </c>
+      <c r="B213">
+        <v>0</v>
+      </c>
+      <c r="D213" t="s">
+        <v>427</v>
       </c>
       <c r="E213" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A214" s="3" t="s">
-        <v>425</v>
-      </c>
-      <c r="B214" s="3">
-        <v>0</v>
-      </c>
-      <c r="C214" s="3"/>
-      <c r="D214" s="3" t="s">
-        <v>426</v>
+      <c r="A214" t="s">
+        <v>429</v>
+      </c>
+      <c r="B214">
+        <v>0</v>
+      </c>
+      <c r="D214" t="s">
+        <v>430</v>
       </c>
       <c r="E214" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A215" t="s">
-        <v>428</v>
-      </c>
-      <c r="B215">
-        <v>0</v>
-      </c>
-      <c r="D215" t="s">
-        <v>429</v>
-      </c>
-      <c r="E215" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A216" t="s">
         <v>431</v>
-      </c>
-      <c r="B216">
-        <v>0</v>
-      </c>
-      <c r="D216" t="s">
-        <v>432</v>
-      </c>
-      <c r="E216" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A217" t="s">
-        <v>434</v>
-      </c>
-      <c r="B217">
-        <v>0</v>
-      </c>
-      <c r="D217" t="s">
-        <v>435</v>
-      </c>
-      <c r="E217" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A218" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="B218" s="3">
-        <v>0</v>
-      </c>
-      <c r="C218" s="3"/>
-      <c r="D218" s="3" t="s">
-        <v>429</v>
-      </c>
-      <c r="E218" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A219" s="3" t="s">
-        <v>438</v>
-      </c>
-      <c r="B219" s="3">
-        <v>0</v>
-      </c>
-      <c r="C219" s="3"/>
-      <c r="D219" s="3" t="s">
-        <v>439</v>
-      </c>
-      <c r="E219" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A220" t="s">
-        <v>441</v>
-      </c>
-      <c r="B220">
-        <v>0</v>
-      </c>
-      <c r="D220" t="s">
-        <v>442</v>
-      </c>
-      <c r="E220" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A221" t="s">
-        <v>444</v>
-      </c>
-      <c r="B221">
-        <v>0</v>
-      </c>
-      <c r="D221" t="s">
-        <v>445</v>
-      </c>
-      <c r="E221" t="s">
-        <v>446</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <sortState ref="A2:E220">
-    <sortCondition ref="A220"/>
+  <sortState ref="A2:E214">
+    <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
use fragments for cookieconsent
</commit_message>
<xml_diff>
--- a/database/seeds/data/fragments.xlsx
+++ b/database/seeds/data/fragments.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/willem/Sites/blender/database/seeds/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/freek/dev/github/blender/database/seeds/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17620" activeTab="1"/>
+    <workbookView xWindow="24800" yWindow="6460" windowWidth="28800" windowHeight="17620"/>
   </bookViews>
   <sheets>
     <sheet name="fragments" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="471">
   <si>
     <t>name</t>
   </si>
@@ -1429,6 +1429,18 @@
   </si>
   <si>
     <t>Systeem</t>
+  </si>
+  <si>
+    <t>cookieConsent.message</t>
+  </si>
+  <si>
+    <t>cookieConsent.agree</t>
+  </si>
+  <si>
+    <t>Voor deze sites gebruiken we cookies om de gebruikservaring te verbeteren. Indien u verder surft gaan we ervan uit dat u cookies toelaat.</t>
+  </si>
+  <si>
+    <t>Ok</t>
   </si>
 </sst>
 </file>
@@ -1784,11 +1796,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z16"/>
+  <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2049,6 +2061,22 @@
         <v>48</v>
       </c>
     </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>467</v>
+      </c>
+      <c r="D17" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>468</v>
+      </c>
+      <c r="D18" t="s">
+        <v>470</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
@@ -2063,8 +2091,8 @@
   </sheetPr>
   <dimension ref="A1:Z216"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D137" sqref="D137"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add sub articles support (#48)
</commit_message>
<xml_diff>
--- a/database/seeds/data/fragments.xlsx
+++ b/database/seeds/data/fragments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24800" yWindow="6460" windowWidth="28800" windowHeight="17620"/>
+    <workbookView xWindow="22400" yWindow="6460" windowWidth="28800" windowHeight="17620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="fragments" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="473">
   <si>
     <t>name</t>
   </si>
@@ -1441,6 +1441,12 @@
   </si>
   <si>
     <t>Ok</t>
+  </si>
+  <si>
+    <t>back.articles.parent_id</t>
+  </si>
+  <si>
+    <t>Sub artikel van</t>
   </si>
 </sst>
 </file>
@@ -1798,9 +1804,9 @@
   </sheetPr>
   <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2089,11 +2095,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z216"/>
+  <dimension ref="A1:Z217"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D137" sqref="D137"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A196" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D215" sqref="D215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4688,6 +4694,17 @@
         <v>431</v>
       </c>
     </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>471</v>
+      </c>
+      <c r="B217">
+        <v>0</v>
+      </c>
+      <c r="D217" t="s">
+        <v>472</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <sortState ref="A2:E214">

</xml_diff>

<commit_message>
add google recaptcha to contact form
</commit_message>
<xml_diff>
--- a/database/seeds/data/fragments.xlsx
+++ b/database/seeds/data/fragments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="6460" windowWidth="28800" windowHeight="17620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="28700"/>
   </bookViews>
   <sheets>
     <sheet name="fragments" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="495">
   <si>
     <t>name</t>
   </si>
@@ -1447,6 +1447,72 @@
   </si>
   <si>
     <t>Sub artikel van</t>
+  </si>
+  <si>
+    <t>form.name</t>
+  </si>
+  <si>
+    <t>form.telephone</t>
+  </si>
+  <si>
+    <t>form.email</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>form.address</t>
+  </si>
+  <si>
+    <t>form.postal</t>
+  </si>
+  <si>
+    <t>Plaatsnaam</t>
+  </si>
+  <si>
+    <t>form.city</t>
+  </si>
+  <si>
+    <t>Opmerkingen</t>
+  </si>
+  <si>
+    <t>contact.button</t>
+  </si>
+  <si>
+    <t>form.fieldsAreRequired</t>
+  </si>
+  <si>
+    <t>Deze velden zijn verplicht</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Telephone</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Postal</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Verstuur</t>
+  </si>
+  <si>
+    <t>Send</t>
+  </si>
+  <si>
+    <t>Required fields</t>
+  </si>
+  <si>
+    <t>contact.remarks</t>
   </si>
 </sst>
 </file>
@@ -1493,11 +1559,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1802,11 +1871,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z18"/>
+  <dimension ref="A1:Z36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2067,7 +2136,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>467</v>
       </c>
@@ -2075,13 +2144,115 @@
         <v>469</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>468</v>
       </c>
       <c r="D18" t="s">
         <v>470</v>
       </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>473</v>
+      </c>
+      <c r="D19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>474</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>475</v>
+      </c>
+      <c r="D21" t="s">
+        <v>476</v>
+      </c>
+      <c r="E21" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>477</v>
+      </c>
+      <c r="D22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>478</v>
+      </c>
+      <c r="D23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>480</v>
+      </c>
+      <c r="D24" t="s">
+        <v>479</v>
+      </c>
+      <c r="E24" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>494</v>
+      </c>
+      <c r="D25" t="s">
+        <v>481</v>
+      </c>
+      <c r="E25" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>482</v>
+      </c>
+      <c r="D26" t="s">
+        <v>491</v>
+      </c>
+      <c r="E26" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>483</v>
+      </c>
+      <c r="D27" t="s">
+        <v>484</v>
+      </c>
+      <c r="E27" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E36" s="4"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -2097,8 +2268,8 @@
   </sheetPr>
   <dimension ref="A1:Z217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A196" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D215" sqref="D215"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add sublayouts; Rearrange front css
</commit_message>
<xml_diff>
--- a/database/seeds/data/fragments.xlsx
+++ b/database/seeds/data/fragments.xlsx
@@ -1530,7 +1530,7 @@
     <t>back.formResponses.mailConfigMissing</t>
   </si>
   <si>
-    <t>Momenteel worden reacties nog niet gemaild omdat er geen bestemming werd ingesteld. Download hier de backup van alle reacties als .xlsx-bestand (Excel).</t>
+    <t xml:space="preserve">Momenteel worden reacties nog niet gemaild omdat er geen bestemming werd ingesteld. </t>
   </si>
 </sst>
 </file>
@@ -2288,7 +2288,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A189" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D220" sqref="D220"/>
+      <selection pane="bottomLeft" activeCell="A228" sqref="A228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Use clearer admin URLs without camelCase
</commit_message>
<xml_diff>
--- a/database/seeds/data/fragments.xlsx
+++ b/database/seeds/data/fragments.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27510"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="502">
   <si>
     <t>name</t>
   </si>
@@ -591,15 +591,9 @@
     <t>back.backUsers.administrator</t>
   </si>
   <si>
-    <t>Administrator</t>
-  </si>
-  <si>
     <t>back.backUsers.automaticCredentialsMailInfo</t>
   </si>
   <si>
-    <t>Zodra je deze nieuwe administrator bewaart, zullen we hem/haar een e-mail sturen met een link om het wachtwoord in te stellen.</t>
-  </si>
-  <si>
     <t>back.backUsers.first_name</t>
   </si>
   <si>
@@ -642,9 +636,6 @@
     <t>back.backUsers.new</t>
   </si>
   <si>
-    <t>Nieuwe administrator</t>
-  </si>
-  <si>
     <t>back.backUsers.password</t>
   </si>
   <si>
@@ -666,15 +657,9 @@
     <t>back.backUsers.save</t>
   </si>
   <si>
-    <t>Bewaar administrator</t>
-  </si>
-  <si>
     <t>back.backUsers.title</t>
   </si>
   <si>
-    <t>Administrators</t>
-  </si>
-  <si>
     <t>back.change</t>
   </si>
   <si>
@@ -1531,6 +1516,24 @@
   </si>
   <si>
     <t xml:space="preserve">Momenteel worden reacties nog niet gemaild omdat er geen bestemming werd ingesteld. </t>
+  </si>
+  <si>
+    <t>Beheerder</t>
+  </si>
+  <si>
+    <t>Zodra je deze nieuwe beheerder bewaart, zullen we hem/haar een e-mail sturen met een link om het wachtwoord in te stellen.</t>
+  </si>
+  <si>
+    <t>Nieuwe beheerder</t>
+  </si>
+  <si>
+    <t>Er is een mail verstuurd waarmee deze beheerder zelf een wachtwoord kan instellen.</t>
+  </si>
+  <si>
+    <t>Bewaar beheerder</t>
+  </si>
+  <si>
+    <t>Beheerders</t>
   </si>
 </sst>
 </file>
@@ -2156,117 +2159,117 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="D17" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="D18" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="D19" t="s">
         <v>69</v>
       </c>
       <c r="E19" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="D20" t="s">
         <v>44</v>
       </c>
       <c r="E20" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="D21" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="E21" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="D22" t="s">
         <v>50</v>
       </c>
       <c r="E22" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="D23" t="s">
         <v>107</v>
       </c>
       <c r="E23" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="D24" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="E24" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="D25" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="E25" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="D26" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="E26" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="D27" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="E27" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
     </row>
     <row r="36" spans="5:5" x14ac:dyDescent="0.2">
@@ -2287,8 +2290,8 @@
   <dimension ref="A1:Z220"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A189" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A228" sqref="A228"/>
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2491,13 +2494,13 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
@@ -2639,7 +2642,7 @@
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="E25" t="s">
         <v>99</v>
@@ -2653,7 +2656,7 @@
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="E26" t="s">
         <v>101</v>
@@ -2876,7 +2879,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -2958,7 +2961,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>153</v>
       </c>
@@ -2969,7 +2972,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>155</v>
       </c>
@@ -2980,7 +2983,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>157</v>
       </c>
@@ -2991,7 +2994,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>159</v>
       </c>
@@ -3002,7 +3005,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>161</v>
       </c>
@@ -3013,7 +3016,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>163</v>
       </c>
@@ -3024,7 +3027,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>164</v>
       </c>
@@ -3035,7 +3038,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>166</v>
       </c>
@@ -3046,1894 +3049,1896 @@
         <v>167</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>464</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="D57" t="s">
+        <v>489</v>
+      </c>
+      <c r="E57" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>168</v>
       </c>
-      <c r="B57">
-        <v>0</v>
-      </c>
-      <c r="D57" t="s">
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="D58" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>170</v>
       </c>
-      <c r="B58">
-        <v>0</v>
-      </c>
-      <c r="D58" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="D59" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>171</v>
       </c>
-      <c r="B59">
-        <v>0</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="D60" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>173</v>
       </c>
-      <c r="B60">
-        <v>0</v>
-      </c>
-      <c r="D60" t="s">
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="D61" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>175</v>
       </c>
-      <c r="B61">
-        <v>0</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="D62" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>177</v>
       </c>
-      <c r="B62">
-        <v>0</v>
-      </c>
-      <c r="D62" t="s">
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="D63" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>179</v>
       </c>
-      <c r="B63">
-        <v>0</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="D64" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>180</v>
-      </c>
-      <c r="B64">
-        <v>0</v>
-      </c>
-      <c r="D64" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B65">
         <v>0</v>
       </c>
       <c r="D65" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B66">
         <v>0</v>
       </c>
       <c r="D66" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>438</v>
+        <v>182</v>
       </c>
       <c r="B67">
         <v>0</v>
       </c>
       <c r="D67" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="B68">
         <v>0</v>
       </c>
       <c r="D68" t="s">
-        <v>117</v>
+        <v>38</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>183</v>
+        <v>432</v>
       </c>
       <c r="B69">
         <v>0</v>
       </c>
       <c r="D69" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B70">
         <v>0</v>
       </c>
       <c r="D70" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B71">
         <v>0</v>
       </c>
       <c r="D71" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>460</v>
+        <v>185</v>
       </c>
       <c r="B72">
         <v>0</v>
       </c>
       <c r="D72" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>440</v>
+        <v>455</v>
       </c>
       <c r="B73">
         <v>0</v>
       </c>
       <c r="D73" t="s">
-        <v>441</v>
+        <v>105</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="B74" s="3">
-        <v>0</v>
-      </c>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3" t="s">
-        <v>129</v>
+      <c r="A74" t="s">
+        <v>435</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="D74" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B75" s="3">
         <v>0</v>
       </c>
       <c r="C75" s="3"/>
       <c r="D75" s="3" t="s">
-        <v>431</v>
+        <v>129</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>186</v>
-      </c>
-      <c r="B76">
-        <v>0</v>
-      </c>
-      <c r="D76" t="s">
-        <v>187</v>
+      <c r="A76" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="B76" s="3">
+        <v>0</v>
+      </c>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B77">
         <v>0</v>
       </c>
       <c r="D77" t="s">
-        <v>189</v>
+        <v>496</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B78">
         <v>0</v>
       </c>
       <c r="D78" t="s">
-        <v>26</v>
+        <v>497</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B79">
         <v>0</v>
       </c>
       <c r="D79" t="s">
-        <v>192</v>
+        <v>26</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B80">
         <v>0</v>
       </c>
       <c r="D80" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B81">
         <v>0</v>
       </c>
       <c r="D81" t="s">
-        <v>29</v>
+        <v>192</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B82">
         <v>0</v>
       </c>
       <c r="D82" t="s">
-        <v>197</v>
+        <v>29</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B83">
         <v>0</v>
       </c>
       <c r="D83" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B84">
         <v>0</v>
       </c>
       <c r="D84" t="s">
-        <v>69</v>
+        <v>197</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B85">
         <v>0</v>
       </c>
       <c r="D85" t="s">
-        <v>202</v>
+        <v>69</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B86">
         <v>0</v>
       </c>
       <c r="D86" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B87">
         <v>0</v>
       </c>
       <c r="D87" t="s">
-        <v>35</v>
+        <v>498</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B88">
         <v>0</v>
       </c>
       <c r="D88" t="s">
-        <v>207</v>
+        <v>35</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B89">
         <v>0</v>
       </c>
       <c r="D89" t="s">
-        <v>38</v>
+        <v>204</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B90">
         <v>0</v>
       </c>
       <c r="D90" t="s">
-        <v>210</v>
+        <v>38</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B91">
         <v>0</v>
       </c>
       <c r="D91" t="s">
-        <v>212</v>
+        <v>499</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B92">
         <v>0</v>
       </c>
       <c r="D92" t="s">
-        <v>214</v>
+        <v>500</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B93">
         <v>0</v>
       </c>
       <c r="D93" t="s">
-        <v>216</v>
+        <v>501</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>442</v>
+        <v>210</v>
       </c>
       <c r="B94">
         <v>0</v>
       </c>
       <c r="D94" t="s">
-        <v>447</v>
+        <v>211</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>217</v>
+        <v>437</v>
       </c>
       <c r="B95">
         <v>0</v>
       </c>
       <c r="D95" t="s">
-        <v>218</v>
+        <v>442</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B96">
         <v>0</v>
       </c>
       <c r="D96" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B97">
         <v>0</v>
       </c>
       <c r="D97" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B98">
         <v>0</v>
       </c>
       <c r="D98" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B99">
         <v>0</v>
       </c>
       <c r="D99" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B100">
         <v>0</v>
       </c>
       <c r="D100" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="B101">
         <v>0</v>
       </c>
       <c r="D101" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B102">
         <v>0</v>
       </c>
       <c r="D102" t="s">
-        <v>439</v>
+        <v>225</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B103">
         <v>0</v>
       </c>
       <c r="D103" t="s">
-        <v>233</v>
+        <v>434</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>234</v>
+        <v>494</v>
       </c>
       <c r="B104">
         <v>0</v>
       </c>
       <c r="D104" t="s">
-        <v>235</v>
+        <v>495</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>444</v>
+        <v>227</v>
       </c>
       <c r="B105">
         <v>0</v>
       </c>
       <c r="D105" t="s">
-        <v>449</v>
+        <v>228</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="B106">
         <v>0</v>
       </c>
       <c r="D106" t="s">
-        <v>69</v>
+        <v>230</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>237</v>
+        <v>439</v>
       </c>
       <c r="B107">
         <v>0</v>
       </c>
       <c r="D107" t="s">
-        <v>238</v>
+        <v>444</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="B108">
         <v>0</v>
       </c>
       <c r="D108" t="s">
-        <v>176</v>
+        <v>69</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="B109">
         <v>0</v>
       </c>
       <c r="D109" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="B110">
         <v>0</v>
       </c>
       <c r="D110" t="s">
-        <v>243</v>
+        <v>176</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="B111">
         <v>0</v>
       </c>
       <c r="D111" t="s">
-        <v>26</v>
+        <v>236</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="B112">
         <v>0</v>
       </c>
       <c r="D112" t="s">
-        <v>194</v>
+        <v>238</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="B113">
         <v>0</v>
       </c>
       <c r="D113" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="B114">
         <v>0</v>
       </c>
       <c r="D114" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="B115">
         <v>0</v>
       </c>
       <c r="D115" t="s">
-        <v>199</v>
+        <v>29</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="B116">
         <v>0</v>
       </c>
       <c r="D116" t="s">
-        <v>250</v>
+        <v>195</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="B117">
         <v>0</v>
       </c>
       <c r="D117" t="s">
-        <v>69</v>
+        <v>197</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="B118">
         <v>0</v>
       </c>
       <c r="D118" t="s">
-        <v>202</v>
+        <v>245</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="B119">
         <v>0</v>
       </c>
       <c r="D119" t="s">
-        <v>254</v>
+        <v>69</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="B120">
         <v>0</v>
       </c>
       <c r="D120" t="s">
-        <v>256</v>
+        <v>200</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B121">
         <v>0</v>
       </c>
       <c r="D121" t="s">
-        <v>210</v>
+        <v>249</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="B122">
         <v>0</v>
       </c>
       <c r="D122" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="B123">
         <v>0</v>
       </c>
       <c r="D123" t="s">
-        <v>261</v>
+        <v>207</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="B124">
         <v>0</v>
       </c>
       <c r="D124" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="B125">
         <v>0</v>
       </c>
       <c r="D125" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="B126">
         <v>0</v>
       </c>
       <c r="D126" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="B127">
         <v>0</v>
       </c>
       <c r="D127" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="B128">
         <v>0</v>
       </c>
       <c r="D128" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="B129">
         <v>0</v>
       </c>
       <c r="D129" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="B130">
         <v>0</v>
       </c>
       <c r="D130" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>443</v>
+        <v>267</v>
       </c>
       <c r="B131">
         <v>0</v>
       </c>
       <c r="D131" t="s">
-        <v>448</v>
+        <v>268</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="B132">
         <v>0</v>
       </c>
       <c r="D132" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>278</v>
+        <v>438</v>
       </c>
       <c r="B133">
         <v>0</v>
       </c>
       <c r="D133" t="s">
-        <v>69</v>
+        <v>443</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>451</v>
+        <v>271</v>
       </c>
       <c r="B134">
         <v>0</v>
       </c>
       <c r="D134" t="s">
-        <v>454</v>
+        <v>272</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>452</v>
+        <v>273</v>
       </c>
       <c r="B135">
         <v>0</v>
       </c>
       <c r="D135" t="s">
-        <v>235</v>
+        <v>69</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>461</v>
+        <v>446</v>
       </c>
       <c r="B136">
         <v>0</v>
       </c>
       <c r="D136" t="s">
-        <v>462</v>
+        <v>449</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>463</v>
+        <v>447</v>
       </c>
       <c r="B137">
         <v>0</v>
       </c>
       <c r="D137" t="s">
-        <v>464</v>
+        <v>230</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="B138">
         <v>0</v>
       </c>
       <c r="D138" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>279</v>
+        <v>458</v>
       </c>
       <c r="B139">
         <v>0</v>
       </c>
       <c r="D139" t="s">
-        <v>158</v>
+        <v>459</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>280</v>
+        <v>456</v>
       </c>
       <c r="B140">
         <v>0</v>
       </c>
       <c r="D140" t="s">
-        <v>160</v>
+        <v>457</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="B141">
         <v>0</v>
       </c>
       <c r="D141" t="s">
-        <v>69</v>
+        <v>158</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="B142">
         <v>0</v>
       </c>
       <c r="D142" t="s">
-        <v>283</v>
+        <v>160</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="B143">
         <v>0</v>
       </c>
       <c r="D143" t="s">
-        <v>285</v>
+        <v>69</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="B144">
         <v>0</v>
       </c>
       <c r="D144" t="s">
-        <v>174</v>
+        <v>278</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="B145">
         <v>0</v>
       </c>
       <c r="D145" t="s">
-        <v>167</v>
+        <v>280</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="B146">
         <v>0</v>
       </c>
       <c r="D146" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B147">
         <v>0</v>
       </c>
       <c r="D147" t="s">
-        <v>495</v>
+        <v>167</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="B148">
         <v>0</v>
       </c>
       <c r="D148" t="s">
-        <v>291</v>
+        <v>169</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="B149">
         <v>0</v>
       </c>
       <c r="D149" t="s">
-        <v>174</v>
+        <v>490</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="B150">
         <v>0</v>
       </c>
       <c r="D150" t="s">
-        <v>176</v>
+        <v>286</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="B151">
         <v>0</v>
       </c>
       <c r="D151" t="s">
-        <v>295</v>
+        <v>174</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="B152">
         <v>0</v>
       </c>
       <c r="D152" t="s">
-        <v>297</v>
+        <v>176</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="B153">
         <v>0</v>
       </c>
       <c r="D153" t="s">
-        <v>24</v>
+        <v>290</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="B154">
         <v>0</v>
       </c>
       <c r="D154" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B155">
         <v>0</v>
       </c>
       <c r="D155" t="s">
-        <v>160</v>
+        <v>24</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="B156">
         <v>0</v>
       </c>
       <c r="D156" t="s">
-        <v>69</v>
+        <v>295</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="B157">
         <v>0</v>
       </c>
       <c r="D157" t="s">
-        <v>304</v>
+        <v>160</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="B158">
         <v>0</v>
       </c>
       <c r="D158" t="s">
-        <v>167</v>
+        <v>69</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="B159">
         <v>0</v>
       </c>
       <c r="D159" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="B160">
         <v>0</v>
       </c>
       <c r="D160" t="s">
-        <v>309</v>
+        <v>167</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="B161">
         <v>0</v>
       </c>
       <c r="D161" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="B162">
         <v>0</v>
       </c>
       <c r="D162" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="B163">
         <v>0</v>
       </c>
       <c r="D163" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>492</v>
+        <v>307</v>
       </c>
       <c r="B164">
         <v>0</v>
       </c>
       <c r="D164" t="s">
-        <v>493</v>
+        <v>308</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="B165">
         <v>0</v>
       </c>
       <c r="D165" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>318</v>
+        <v>491</v>
       </c>
       <c r="B166">
         <v>0</v>
       </c>
       <c r="D166" t="s">
-        <v>319</v>
+        <v>493</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>320</v>
+        <v>487</v>
       </c>
       <c r="B167">
         <v>0</v>
       </c>
       <c r="D167" t="s">
-        <v>321</v>
+        <v>488</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="B168">
         <v>0</v>
       </c>
       <c r="D168" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="B169">
         <v>0</v>
       </c>
       <c r="D169" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="B170">
         <v>0</v>
       </c>
       <c r="D170" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="B171">
         <v>0</v>
       </c>
       <c r="D171" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="B172">
         <v>0</v>
       </c>
       <c r="D172" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="B173">
         <v>0</v>
       </c>
       <c r="D173" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="B174">
         <v>0</v>
       </c>
       <c r="D174" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="B175">
         <v>0</v>
       </c>
       <c r="D175" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="B176">
         <v>0</v>
       </c>
       <c r="D176" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="B177">
         <v>0</v>
       </c>
       <c r="D177" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="B178">
         <v>0</v>
       </c>
       <c r="D178" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="B179">
         <v>0</v>
       </c>
       <c r="D179" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="B180">
         <v>0</v>
       </c>
       <c r="D180" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="B181">
         <v>0</v>
       </c>
       <c r="D181" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
       <c r="B182">
         <v>0</v>
       </c>
       <c r="D182" t="s">
-        <v>269</v>
+        <v>340</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="B183">
         <v>0</v>
       </c>
       <c r="D183" t="s">
-        <v>69</v>
+        <v>342</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="B184">
         <v>0</v>
       </c>
       <c r="D184" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="B185">
         <v>0</v>
       </c>
       <c r="D185" t="s">
-        <v>167</v>
+        <v>264</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="B186">
         <v>0</v>
       </c>
       <c r="D186" t="s">
-        <v>356</v>
+        <v>69</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="B187">
         <v>0</v>
       </c>
       <c r="D187" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="B188">
         <v>0</v>
       </c>
       <c r="D188" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="B189">
         <v>0</v>
       </c>
       <c r="D189" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="B190">
         <v>0</v>
       </c>
       <c r="D190" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="B191">
         <v>0</v>
       </c>
       <c r="D191" t="s">
-        <v>365</v>
+        <v>174</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>445</v>
+        <v>355</v>
       </c>
       <c r="B192">
         <v>0</v>
       </c>
       <c r="D192" t="s">
-        <v>194</v>
+        <v>356</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>446</v>
+        <v>357</v>
       </c>
       <c r="B193">
         <v>0</v>
       </c>
       <c r="D193" t="s">
-        <v>202</v>
+        <v>358</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="B194">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D194" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>368</v>
+        <v>440</v>
       </c>
       <c r="B195">
         <v>0</v>
       </c>
       <c r="D195" t="s">
-        <v>369</v>
-      </c>
-      <c r="E195" t="s">
-        <v>370</v>
+        <v>192</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>371</v>
+        <v>441</v>
       </c>
       <c r="B196">
         <v>0</v>
       </c>
       <c r="D196" t="s">
-        <v>372</v>
-      </c>
-      <c r="E196" t="s">
-        <v>373</v>
+        <v>200</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>374</v>
+        <v>361</v>
       </c>
       <c r="B197">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D197" t="s">
-        <v>375</v>
-      </c>
-      <c r="E197" t="s">
-        <v>376</v>
+        <v>362</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>377</v>
+        <v>363</v>
       </c>
       <c r="B198">
         <v>0</v>
       </c>
       <c r="D198" t="s">
-        <v>378</v>
+        <v>364</v>
       </c>
       <c r="E198" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>380</v>
+        <v>366</v>
       </c>
       <c r="B199">
         <v>0</v>
       </c>
       <c r="D199" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
       <c r="E199" t="s">
-        <v>382</v>
+        <v>368</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
       <c r="B200">
         <v>0</v>
       </c>
       <c r="D200" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
       <c r="E200" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>386</v>
+        <v>372</v>
       </c>
       <c r="B201">
         <v>0</v>
       </c>
       <c r="D201" t="s">
-        <v>433</v>
+        <v>373</v>
       </c>
       <c r="E201" t="s">
-        <v>435</v>
+        <v>374</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="B202">
         <v>0</v>
       </c>
       <c r="D202" t="s">
-        <v>436</v>
+        <v>376</v>
       </c>
       <c r="E202" t="s">
-        <v>434</v>
+        <v>377</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="B203">
         <v>0</v>
       </c>
       <c r="D203" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="E203" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="B204">
         <v>0</v>
       </c>
       <c r="D204" t="s">
-        <v>392</v>
+        <v>428</v>
       </c>
       <c r="E204" t="s">
-        <v>393</v>
+        <v>430</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
       <c r="B205">
         <v>0</v>
       </c>
       <c r="D205" t="s">
-        <v>395</v>
+        <v>431</v>
       </c>
       <c r="E205" t="s">
-        <v>396</v>
+        <v>429</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" s="2" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
       <c r="B206" s="2">
         <v>0</v>
       </c>
       <c r="C206" s="2"/>
       <c r="D206" s="2" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="E206" t="s">
-        <v>399</v>
+        <v>385</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" s="2" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
       <c r="B207" s="2">
         <v>0</v>
       </c>
       <c r="C207" s="2"/>
       <c r="D207" s="2" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
       <c r="E207" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
       <c r="B208">
         <v>0</v>
       </c>
       <c r="D208" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c r="E208" t="s">
-        <v>404</v>
+        <v>391</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" s="3" t="s">
-        <v>405</v>
+        <v>392</v>
       </c>
       <c r="B209" s="3">
         <v>0</v>
       </c>
       <c r="C209" s="3"/>
       <c r="D209" s="3" t="s">
-        <v>406</v>
+        <v>393</v>
       </c>
       <c r="E209" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" s="3" t="s">
-        <v>408</v>
+        <v>395</v>
       </c>
       <c r="B210" s="3">
         <v>0</v>
       </c>
       <c r="C210" s="3"/>
       <c r="D210" s="3" t="s">
-        <v>409</v>
+        <v>396</v>
       </c>
       <c r="E210" t="s">
-        <v>410</v>
+        <v>397</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
+        <v>398</v>
+      </c>
+      <c r="B211">
+        <v>0</v>
+      </c>
+      <c r="D211" t="s">
+        <v>396</v>
+      </c>
+      <c r="E211" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A212" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="B212" s="3">
+        <v>0</v>
+      </c>
+      <c r="C212" s="3"/>
+      <c r="D212" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="E212" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A213" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="B213" s="3">
+        <v>0</v>
+      </c>
+      <c r="C213" s="3"/>
+      <c r="D213" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="E213" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>406</v>
+      </c>
+      <c r="B214">
+        <v>0</v>
+      </c>
+      <c r="D214" t="s">
+        <v>407</v>
+      </c>
+      <c r="E214" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>409</v>
+      </c>
+      <c r="B215">
+        <v>0</v>
+      </c>
+      <c r="D215" t="s">
+        <v>410</v>
+      </c>
+      <c r="E215" t="s">
         <v>411</v>
-      </c>
-      <c r="B211">
-        <v>0</v>
-      </c>
-      <c r="D211" t="s">
-        <v>412</v>
-      </c>
-      <c r="E211" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A212" t="s">
-        <v>414</v>
-      </c>
-      <c r="B212">
-        <v>0</v>
-      </c>
-      <c r="D212" t="s">
-        <v>415</v>
-      </c>
-      <c r="E212" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A213" t="s">
-        <v>417</v>
-      </c>
-      <c r="B213">
-        <v>0</v>
-      </c>
-      <c r="D213" t="s">
-        <v>418</v>
-      </c>
-      <c r="E213" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A214" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="B214" s="3">
-        <v>0</v>
-      </c>
-      <c r="C214" s="3"/>
-      <c r="D214" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="E214" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A215" s="3" t="s">
-        <v>421</v>
-      </c>
-      <c r="B215" s="3">
-        <v>0</v>
-      </c>
-      <c r="C215" s="3"/>
-      <c r="D215" s="3" t="s">
-        <v>422</v>
-      </c>
-      <c r="E215" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="B216">
         <v>0</v>
       </c>
       <c r="D216" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="E216" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A217" t="s">
-        <v>427</v>
-      </c>
-      <c r="B217">
-        <v>0</v>
-      </c>
-      <c r="D217" t="s">
-        <v>428</v>
+      <c r="A217" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B217" s="3">
+        <v>0</v>
+      </c>
+      <c r="C217" s="3"/>
+      <c r="D217" s="3" t="s">
+        <v>407</v>
       </c>
       <c r="E217" t="s">
-        <v>429</v>
+        <v>408</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A218" t="s">
-        <v>469</v>
-      </c>
-      <c r="B218">
-        <v>0</v>
-      </c>
-      <c r="D218" t="s">
-        <v>494</v>
+      <c r="A218" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="B218" s="3">
+        <v>0</v>
+      </c>
+      <c r="C218" s="3"/>
+      <c r="D218" s="3" t="s">
+        <v>417</v>
       </c>
       <c r="E218" t="s">
-        <v>497</v>
+        <v>418</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>496</v>
+        <v>419</v>
       </c>
       <c r="B219">
         <v>0</v>
       </c>
       <c r="D219" t="s">
-        <v>498</v>
+        <v>420</v>
+      </c>
+      <c r="E219" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>499</v>
+        <v>422</v>
       </c>
       <c r="B220">
         <v>0</v>
       </c>
       <c r="D220" t="s">
-        <v>500</v>
+        <v>423</v>
+      </c>
+      <c r="E220" t="s">
+        <v>424</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <sortState ref="A2:E214">
-    <sortCondition ref="A2"/>
+  <sortState ref="A2:Z220">
+    <sortCondition ref="A2:A220"/>
   </sortState>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Added back to index links
</commit_message>
<xml_diff>
--- a/database/seeds/data/fragments.xlsx
+++ b/database/seeds/data/fragments.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="509">
   <si>
     <t>name</t>
   </si>
@@ -1552,6 +1552,12 @@
   </si>
   <si>
     <t>administrators.title</t>
+  </si>
+  <si>
+    <t>backToIndex</t>
+  </si>
+  <si>
+    <t>Terug naar overzicht</t>
   </si>
 </sst>
 </file>
@@ -1598,7 +1604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1607,6 +1613,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2387,11 +2394,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA224"/>
+  <dimension ref="A1:AA225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B195" sqref="B195"/>
+      <pane ySplit="1" topLeftCell="A172" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A225" sqref="A225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5754,6 +5761,20 @@
         <v>456</v>
       </c>
     </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>338</v>
+      </c>
+      <c r="B225" s="6" t="s">
+        <v>507</v>
+      </c>
+      <c r="C225" s="6">
+        <v>0</v>
+      </c>
+      <c r="E225" s="6" t="s">
+        <v>508</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A1:F224"/>

</xml_diff>

<commit_message>
Add frontlink on logout
</commit_message>
<xml_diff>
--- a/database/seeds/data/fragments.xlsx
+++ b/database/seeds/data/fragments.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27715"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiandedeyne/Sites/blender/database/seeds/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/willem/Sites/blender/database/seeds/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="460" windowWidth="25600" windowHeight="21060" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28260" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="fragments" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="511">
   <si>
     <t>name</t>
   </si>
@@ -1558,6 +1558,12 @@
   </si>
   <si>
     <t>Terug naar overzicht</t>
+  </si>
+  <si>
+    <t>auth.frontLink</t>
+  </si>
+  <si>
+    <t>Publieke site</t>
   </si>
 </sst>
 </file>
@@ -2394,11 +2400,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA225"/>
+  <dimension ref="A1:AA226"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A172" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A225" sqref="A225"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5775,6 +5781,20 @@
         <v>508</v>
       </c>
     </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>338</v>
+      </c>
+      <c r="B226" s="6" t="s">
+        <v>509</v>
+      </c>
+      <c r="C226" s="6">
+        <v>0</v>
+      </c>
+      <c r="E226" s="6" t="s">
+        <v>510</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A1:F224"/>

</xml_diff>

<commit_message>
Layout mails; Use @spatie/scss on front
</commit_message>
<xml_diff>
--- a/database/seeds/data/fragments.xlsx
+++ b/database/seeds/data/fragments.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27907"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28260" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28260"/>
   </bookViews>
   <sheets>
     <sheet name="fragments" sheetId="1" r:id="rId1"/>
     <sheet name="hidden" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">hidden!$A$1:$F$224</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">hidden!$A$1:$F$215</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="487">
   <si>
     <t>name</t>
   </si>
@@ -174,9 +174,6 @@
     <t>Naam</t>
   </si>
   <si>
-    <t>Ce lien est valable jusqu'au</t>
-  </si>
-  <si>
     <t>Je bent nu uitgelogd.</t>
   </si>
   <si>
@@ -219,30 +216,6 @@
     <t>auth.passwordConfirm</t>
   </si>
   <si>
-    <t>Beste</t>
-  </si>
-  <si>
-    <t>Che(è)r(e)</t>
-  </si>
-  <si>
-    <t>Je hebt toegang gekregen tot</t>
-  </si>
-  <si>
-    <t>Deze link is geldig tot</t>
-  </si>
-  <si>
-    <t>Nous avons reçu une demande de changer votre mot de passe</t>
-  </si>
-  <si>
-    <t>Dans le cas où vous avez fait la demande noot une réinitialisation de mot de passe , ignorez ce e-mail.</t>
-  </si>
-  <si>
-    <t>Wachtwoord wijzigen</t>
-  </si>
-  <si>
-    <t>Changer le mot de passe</t>
-  </si>
-  <si>
     <t>Wachtwoord instellen</t>
   </si>
   <si>
@@ -726,18 +699,6 @@
     <t>Terug naar login</t>
   </si>
   <si>
-    <t>Uw wachtwoord op</t>
-  </si>
-  <si>
-    <t>Accès à</t>
-  </si>
-  <si>
-    <t>Votre mot de passe sur</t>
-  </si>
-  <si>
-    <t>Toegang tot</t>
-  </si>
-  <si>
     <t>De reacties worden standaard gemaild naar &lt;strong&gt;:recipients&lt;/strong&gt;. Download hier de backup van alle reacties als .xlsx-bestand (Excel).</t>
   </si>
   <si>
@@ -762,12 +723,6 @@
     <t>Uitloggen</t>
   </si>
   <si>
-    <t>We ontvingen je vraag om je wachtwoord te wijzigen op</t>
-  </si>
-  <si>
-    <t>Was het een foutieve aanvraag? Negeer dan deze e-mail, je oude wachtwoord blijft gewoon werken.</t>
-  </si>
-  <si>
     <t>Profielen</t>
   </si>
   <si>
@@ -969,27 +924,6 @@
     <t>passwordConfirm</t>
   </si>
   <si>
-    <t>passwordMail.compellation</t>
-  </si>
-  <si>
-    <t>passwordMail.linkValidUntil</t>
-  </si>
-  <si>
-    <t>passwordMail.newUser.intro</t>
-  </si>
-  <si>
-    <t>passwordMail.newUser.resetButton</t>
-  </si>
-  <si>
-    <t>passwordMail.oldUser.intro</t>
-  </si>
-  <si>
-    <t>passwordMail.oldUser.outro</t>
-  </si>
-  <si>
-    <t>passwordMail.oldUser.resetButton</t>
-  </si>
-  <si>
     <t>register</t>
   </si>
   <si>
@@ -1327,12 +1261,6 @@
   </si>
   <si>
     <t>sent</t>
-  </si>
-  <si>
-    <t>subjectEmail</t>
-  </si>
-  <si>
-    <t>subjectEmailNewUser</t>
   </si>
   <si>
     <t>throttle</t>
@@ -1926,7 +1854,7 @@
   </sheetPr>
   <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
     </sheetView>
@@ -1943,10 +1871,10 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1984,10 +1912,10 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="B2" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -2001,10 +1929,10 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="B3" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2018,10 +1946,10 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="B4" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -2035,10 +1963,10 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="B5" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -2052,10 +1980,10 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="B6" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -2069,10 +1997,10 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="B7" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2086,10 +2014,10 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="B8" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -2103,10 +2031,10 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="B9" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -2120,10 +2048,10 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="B10" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -2137,10 +2065,10 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="B11" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -2154,10 +2082,10 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="B12" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -2171,10 +2099,10 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="B13" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -2188,10 +2116,10 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="B14" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -2205,10 +2133,10 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>259</v>
+      </c>
+      <c r="B15" t="s">
         <v>274</v>
-      </c>
-      <c r="B15" t="s">
-        <v>289</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -2222,10 +2150,10 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="B16" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -2239,29 +2167,29 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="B17" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="E17" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="B18" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="E18" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
@@ -2270,119 +2198,119 @@
         <v>46</v>
       </c>
       <c r="F19" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="B20" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="E20" t="s">
         <v>30</v>
       </c>
       <c r="F20" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="B21" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="E21" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="F21" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="B22" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="E22" t="s">
         <v>34</v>
       </c>
       <c r="F22" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="B23" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="E23" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="F23" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="B24" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="E24" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="F24" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="B25" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="E25" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="F25" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="B26" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="E26" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="F26" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="B27" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="E27" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="F27" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
     </row>
     <row r="36" spans="6:6" x14ac:dyDescent="0.2">
@@ -2400,11 +2328,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA226"/>
+  <dimension ref="A1:AA217"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A153" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A193" sqref="A193:XFD194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2419,10 +2347,10 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2460,10 +2388,10 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B2" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -2474,10 +2402,10 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B3" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2491,10 +2419,10 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B4" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -2505,10 +2433,10 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B5" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -2519,10 +2447,10 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B6" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -2536,10 +2464,10 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B7" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -2550,10 +2478,10 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B8" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -2564,10 +2492,10 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B9" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -2581,10 +2509,10 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B10" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -2598,10 +2526,10 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B11" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -2612,109 +2540,109 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B12" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" t="s">
         <v>48</v>
-      </c>
-      <c r="F12" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B13" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="E13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" t="s">
         <v>51</v>
-      </c>
-      <c r="F13" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B14" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B16" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="E16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" t="s">
         <v>54</v>
-      </c>
-      <c r="F16" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B17" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="E17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" t="s">
         <v>56</v>
-      </c>
-      <c r="F17" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B18" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -2725,27 +2653,27 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B19" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="E19" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" t="s">
         <v>59</v>
-      </c>
-      <c r="F19" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B20" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -2759,10 +2687,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B21" t="s">
-        <v>312</v>
+        <v>278</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -2770,33 +2698,27 @@
       <c r="E21" t="s">
         <v>62</v>
       </c>
-      <c r="F21" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B22" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>65</v>
-      </c>
-      <c r="F22" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>283</v>
+      </c>
+      <c r="B23" t="s">
         <v>298</v>
-      </c>
-      <c r="B23" t="s">
-        <v>314</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -2804,259 +2726,268 @@
       <c r="E23" t="s">
         <v>64</v>
       </c>
+      <c r="F23" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B24" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>70</v>
+        <v>66</v>
+      </c>
+      <c r="F24" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B25" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>243</v>
+        <v>69</v>
       </c>
       <c r="F25" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B26" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>244</v>
+        <v>71</v>
       </c>
       <c r="F26" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B27" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="F27" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B28" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>71</v>
+        <v>77</v>
+      </c>
+      <c r="F28" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B29" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="C29">
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>72</v>
+        <v>80</v>
+      </c>
+      <c r="F29" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B30" t="s">
-        <v>320</v>
+        <v>305</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F30" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B31" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="E31" t="s">
+        <v>74</v>
+      </c>
+      <c r="F31" t="s">
         <v>75</v>
-      </c>
-      <c r="F31" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B32" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F32" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B33" t="s">
-        <v>323</v>
+        <v>274</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="F33" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B34" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>83</v>
-      </c>
-      <c r="F34" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B35" t="s">
-        <v>325</v>
+        <v>309</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="F35" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B36" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="E36" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="F36" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B37" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F37" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B38" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="F38" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B39" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -3070,2066 +3001,2048 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B40" t="s">
-        <v>289</v>
+        <v>314</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="E40" t="s">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="F40" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B41" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>70</v>
+        <v>95</v>
+      </c>
+      <c r="F41" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>298</v>
+        <v>316</v>
       </c>
       <c r="B42" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>52</v>
-      </c>
-      <c r="F42" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>298</v>
+        <v>316</v>
       </c>
       <c r="B43" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>73</v>
-      </c>
-      <c r="F43" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>298</v>
+        <v>316</v>
       </c>
       <c r="B44" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="C44">
         <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>89</v>
-      </c>
-      <c r="F44" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>298</v>
+        <v>316</v>
       </c>
       <c r="B45" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
       <c r="C45">
         <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>98</v>
-      </c>
-      <c r="F45" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>298</v>
+        <v>316</v>
       </c>
       <c r="B46" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="C46">
         <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>100</v>
-      </c>
-      <c r="F46" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>298</v>
+        <v>316</v>
       </c>
       <c r="B47" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
       <c r="C47">
         <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>102</v>
-      </c>
-      <c r="F47" t="s">
-        <v>103</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>298</v>
+        <v>316</v>
       </c>
       <c r="B48" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
       <c r="C48">
         <v>0</v>
       </c>
       <c r="E48" t="s">
-        <v>104</v>
-      </c>
-      <c r="F48" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B49" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="C49">
         <v>0</v>
       </c>
       <c r="E49" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B50" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="C50">
         <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B51" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
       <c r="C51">
         <v>0</v>
       </c>
       <c r="E51" t="s">
-        <v>108</v>
+        <v>249</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B52" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="C52">
         <v>0</v>
       </c>
       <c r="E52" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B53" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="C53">
         <v>0</v>
       </c>
       <c r="E53" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B54" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
       <c r="C54">
         <v>0</v>
       </c>
       <c r="E54" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B55" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
       <c r="C55">
         <v>0</v>
       </c>
       <c r="E55" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B56" t="s">
-        <v>346</v>
+        <v>39</v>
       </c>
       <c r="C56">
         <v>0</v>
       </c>
       <c r="E56" t="s">
-        <v>112</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B57" t="s">
-        <v>347</v>
+        <v>41</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
       <c r="E57" t="s">
-        <v>113</v>
+        <v>42</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B58" t="s">
-        <v>348</v>
+        <v>49</v>
       </c>
       <c r="C58">
         <v>0</v>
       </c>
       <c r="E58" t="s">
-        <v>264</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B59" t="s">
-        <v>349</v>
+        <v>57</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
       <c r="E59" t="s">
-        <v>114</v>
+        <v>24</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B60" t="s">
-        <v>350</v>
+        <v>60</v>
       </c>
       <c r="C60">
         <v>0</v>
       </c>
       <c r="E60" t="s">
-        <v>115</v>
+        <v>26</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B61" t="s">
-        <v>351</v>
+        <v>68</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
       <c r="E61" t="s">
-        <v>116</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B62" t="s">
-        <v>352</v>
+        <v>73</v>
       </c>
       <c r="C62">
         <v>0</v>
       </c>
       <c r="E62" t="s">
-        <v>117</v>
+        <v>74</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B63" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
       <c r="E63" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B64" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="C64">
         <v>0</v>
       </c>
       <c r="E64" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B65" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="C65">
         <v>0</v>
       </c>
       <c r="E65" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B66" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="C66">
         <v>0</v>
       </c>
       <c r="E66" t="s">
-        <v>24</v>
+        <v>223</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>338</v>
-      </c>
-      <c r="B67" t="s">
-        <v>61</v>
-      </c>
-      <c r="C67">
-        <v>0</v>
-      </c>
-      <c r="E67" t="s">
-        <v>26</v>
+        <v>316</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C67" s="3">
+        <v>0</v>
+      </c>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>338</v>
-      </c>
-      <c r="B68" t="s">
-        <v>77</v>
-      </c>
-      <c r="C68">
-        <v>0</v>
-      </c>
-      <c r="E68" t="s">
-        <v>78</v>
+        <v>316</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C68" s="3">
+        <v>0</v>
+      </c>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B69" t="s">
-        <v>82</v>
+        <v>466</v>
       </c>
       <c r="C69">
         <v>0</v>
       </c>
       <c r="E69" t="s">
-        <v>83</v>
+        <v>109</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B70" t="s">
-        <v>85</v>
+        <v>467</v>
       </c>
       <c r="C70">
         <v>0</v>
       </c>
       <c r="E70" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B71" t="s">
-        <v>88</v>
+        <v>468</v>
       </c>
       <c r="C71">
         <v>0</v>
       </c>
       <c r="E71" t="s">
-        <v>89</v>
+        <v>18</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B72" t="s">
-        <v>94</v>
+        <v>469</v>
       </c>
       <c r="C72">
         <v>0</v>
       </c>
       <c r="E72" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B73" t="s">
-        <v>95</v>
+        <v>470</v>
       </c>
       <c r="C73">
         <v>0</v>
       </c>
       <c r="E73" t="s">
-        <v>236</v>
+        <v>112</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>338</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C74" s="3">
-        <v>0</v>
-      </c>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3" t="s">
-        <v>89</v>
+        <v>316</v>
+      </c>
+      <c r="B74" t="s">
+        <v>471</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="E74" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>338</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C75" s="3">
-        <v>0</v>
-      </c>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3" t="s">
-        <v>230</v>
+        <v>316</v>
+      </c>
+      <c r="B75" t="s">
+        <v>472</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="E75" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B76" t="s">
-        <v>490</v>
+        <v>473</v>
       </c>
       <c r="C76">
         <v>0</v>
       </c>
       <c r="E76" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B77" t="s">
-        <v>491</v>
+        <v>474</v>
       </c>
       <c r="C77">
         <v>0</v>
       </c>
       <c r="E77" t="s">
-        <v>119</v>
+        <v>46</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B78" t="s">
-        <v>492</v>
+        <v>475</v>
       </c>
       <c r="C78">
         <v>0</v>
       </c>
       <c r="E78" t="s">
-        <v>18</v>
+        <v>115</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B79" t="s">
-        <v>493</v>
+        <v>476</v>
       </c>
       <c r="C79">
         <v>0</v>
       </c>
       <c r="E79" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B80" t="s">
-        <v>494</v>
+        <v>477</v>
       </c>
       <c r="C80">
         <v>0</v>
       </c>
       <c r="E80" t="s">
-        <v>121</v>
+        <v>24</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B81" t="s">
-        <v>495</v>
+        <v>478</v>
       </c>
       <c r="C81">
         <v>0</v>
       </c>
       <c r="E81" t="s">
-        <v>20</v>
+        <v>117</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B82" t="s">
-        <v>496</v>
+        <v>479</v>
       </c>
       <c r="C82">
         <v>0</v>
       </c>
       <c r="E82" t="s">
-        <v>122</v>
+        <v>26</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B83" t="s">
-        <v>497</v>
+        <v>480</v>
       </c>
       <c r="C83">
         <v>0</v>
       </c>
       <c r="E83" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B84" t="s">
-        <v>498</v>
+        <v>481</v>
       </c>
       <c r="C84">
         <v>0</v>
       </c>
       <c r="E84" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B85" t="s">
-        <v>499</v>
+        <v>482</v>
       </c>
       <c r="C85">
         <v>0</v>
       </c>
       <c r="E85" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B86" t="s">
-        <v>500</v>
+        <v>331</v>
       </c>
       <c r="C86">
         <v>0</v>
       </c>
       <c r="E86" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B87" t="s">
-        <v>501</v>
+        <v>332</v>
       </c>
       <c r="C87">
         <v>0</v>
       </c>
       <c r="E87" t="s">
-        <v>24</v>
+        <v>224</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B88" t="s">
-        <v>502</v>
+        <v>333</v>
       </c>
       <c r="C88">
         <v>0</v>
       </c>
       <c r="E88" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B89" t="s">
-        <v>503</v>
+        <v>334</v>
       </c>
       <c r="C89">
         <v>0</v>
       </c>
       <c r="E89" t="s">
-        <v>26</v>
+        <v>123</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B90" t="s">
-        <v>504</v>
+        <v>335</v>
       </c>
       <c r="C90">
         <v>0</v>
       </c>
       <c r="E90" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B91" t="s">
-        <v>505</v>
+        <v>336</v>
       </c>
       <c r="C91">
         <v>0</v>
       </c>
       <c r="E91" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B92" t="s">
-        <v>506</v>
+        <v>337</v>
       </c>
       <c r="C92">
         <v>0</v>
       </c>
       <c r="E92" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
+        <v>316</v>
+      </c>
+      <c r="B93" t="s">
         <v>338</v>
       </c>
-      <c r="B93" t="s">
-        <v>353</v>
-      </c>
       <c r="C93">
         <v>0</v>
       </c>
       <c r="E93" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B94" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="C94">
         <v>0</v>
       </c>
       <c r="E94" t="s">
-        <v>237</v>
+        <v>128</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B95" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="C95">
         <v>0</v>
       </c>
       <c r="E95" t="s">
-        <v>131</v>
+        <v>222</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B96" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
       <c r="C96">
         <v>0</v>
       </c>
       <c r="E96" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B97" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="C97">
         <v>0</v>
       </c>
       <c r="E97" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B98" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="C98">
         <v>0</v>
       </c>
       <c r="E98" t="s">
-        <v>134</v>
+        <v>226</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B99" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="C99">
         <v>0</v>
       </c>
       <c r="E99" t="s">
-        <v>135</v>
+        <v>46</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B100" t="s">
-        <v>360</v>
+        <v>345</v>
       </c>
       <c r="C100">
         <v>0</v>
       </c>
       <c r="E100" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B101" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
       <c r="C101">
         <v>0</v>
       </c>
       <c r="E101" t="s">
-        <v>137</v>
+        <v>107</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B102" t="s">
-        <v>362</v>
+        <v>347</v>
       </c>
       <c r="C102">
         <v>0</v>
       </c>
       <c r="E102" t="s">
-        <v>235</v>
+        <v>132</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B103" t="s">
-        <v>363</v>
+        <v>451</v>
       </c>
       <c r="C103">
         <v>0</v>
       </c>
       <c r="E103" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B104" t="s">
-        <v>364</v>
+        <v>452</v>
       </c>
       <c r="C104">
         <v>0</v>
       </c>
       <c r="E104" t="s">
-        <v>139</v>
+        <v>18</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B105" t="s">
-        <v>365</v>
+        <v>453</v>
       </c>
       <c r="C105">
         <v>0</v>
       </c>
       <c r="E105" t="s">
-        <v>239</v>
+        <v>112</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B106" t="s">
-        <v>366</v>
+        <v>454</v>
       </c>
       <c r="C106">
         <v>0</v>
       </c>
       <c r="E106" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B107" t="s">
-        <v>367</v>
+        <v>455</v>
       </c>
       <c r="C107">
         <v>0</v>
       </c>
       <c r="E107" t="s">
-        <v>140</v>
+        <v>113</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B108" t="s">
-        <v>368</v>
+        <v>456</v>
       </c>
       <c r="C108">
         <v>0</v>
       </c>
       <c r="E108" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B109" t="s">
-        <v>369</v>
+        <v>457</v>
       </c>
       <c r="C109">
         <v>0</v>
       </c>
       <c r="E109" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B110" t="s">
-        <v>475</v>
+        <v>458</v>
       </c>
       <c r="C110">
         <v>0</v>
       </c>
       <c r="E110" t="s">
-        <v>142</v>
+        <v>46</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B111" t="s">
-        <v>476</v>
+        <v>459</v>
       </c>
       <c r="C111">
         <v>0</v>
       </c>
       <c r="E111" t="s">
-        <v>18</v>
+        <v>115</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B112" t="s">
-        <v>477</v>
+        <v>460</v>
       </c>
       <c r="C112">
         <v>0</v>
       </c>
       <c r="E112" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B113" t="s">
-        <v>478</v>
+        <v>461</v>
       </c>
       <c r="C113">
         <v>0</v>
       </c>
       <c r="E113" t="s">
-        <v>20</v>
+        <v>136</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B114" t="s">
-        <v>479</v>
+        <v>462</v>
       </c>
       <c r="C114">
         <v>0</v>
       </c>
       <c r="E114" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B115" t="s">
-        <v>480</v>
+        <v>463</v>
       </c>
       <c r="C115">
         <v>0</v>
       </c>
       <c r="E115" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B116" t="s">
-        <v>481</v>
+        <v>464</v>
       </c>
       <c r="C116">
         <v>0</v>
       </c>
       <c r="E116" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B117" t="s">
-        <v>482</v>
+        <v>465</v>
       </c>
       <c r="C117">
         <v>0</v>
       </c>
       <c r="E117" t="s">
-        <v>46</v>
+        <v>139</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B118" t="s">
-        <v>483</v>
+        <v>348</v>
       </c>
       <c r="C118">
         <v>0</v>
       </c>
       <c r="E118" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B119" t="s">
-        <v>484</v>
+        <v>349</v>
       </c>
       <c r="C119">
         <v>0</v>
       </c>
       <c r="E119" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B120" t="s">
-        <v>485</v>
+        <v>350</v>
       </c>
       <c r="C120">
         <v>0</v>
       </c>
       <c r="E120" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B121" t="s">
-        <v>486</v>
+        <v>351</v>
       </c>
       <c r="C121">
         <v>0</v>
       </c>
       <c r="E121" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B122" t="s">
-        <v>487</v>
+        <v>352</v>
       </c>
       <c r="C122">
         <v>0</v>
       </c>
       <c r="E122" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B123" t="s">
-        <v>488</v>
+        <v>353</v>
       </c>
       <c r="C123">
         <v>0</v>
       </c>
       <c r="E123" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B124" t="s">
-        <v>489</v>
+        <v>354</v>
       </c>
       <c r="C124">
         <v>0</v>
       </c>
       <c r="E124" t="s">
-        <v>148</v>
+        <v>225</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B125" t="s">
-        <v>370</v>
+        <v>355</v>
       </c>
       <c r="C125">
         <v>0</v>
       </c>
       <c r="E125" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B126" t="s">
-        <v>371</v>
+        <v>0</v>
       </c>
       <c r="C126">
         <v>0</v>
       </c>
       <c r="E126" t="s">
-        <v>150</v>
+        <v>46</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B127" t="s">
-        <v>372</v>
+        <v>356</v>
       </c>
       <c r="C127">
         <v>0</v>
       </c>
       <c r="E127" t="s">
-        <v>151</v>
+        <v>228</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B128" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
       <c r="C128">
         <v>0</v>
       </c>
       <c r="E128" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B129" t="s">
-        <v>374</v>
+        <v>358</v>
       </c>
       <c r="C129">
         <v>0</v>
       </c>
       <c r="E129" t="s">
-        <v>153</v>
+        <v>230</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B130" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="C130">
         <v>0</v>
       </c>
       <c r="E130" t="s">
-        <v>154</v>
+        <v>231</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B131" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="C131">
         <v>0</v>
       </c>
       <c r="E131" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B132" t="s">
-        <v>377</v>
+        <v>438</v>
       </c>
       <c r="C132">
         <v>0</v>
       </c>
       <c r="E132" t="s">
-        <v>155</v>
+        <v>99</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B133" t="s">
-        <v>0</v>
+        <v>439</v>
       </c>
       <c r="C133">
         <v>0</v>
       </c>
       <c r="E133" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B134" t="s">
-        <v>378</v>
+        <v>440</v>
       </c>
       <c r="C134">
         <v>0</v>
       </c>
       <c r="E134" t="s">
-        <v>241</v>
+        <v>46</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B135" t="s">
-        <v>379</v>
+        <v>441</v>
       </c>
       <c r="C135">
         <v>0</v>
       </c>
       <c r="E135" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B136" t="s">
-        <v>380</v>
+        <v>442</v>
       </c>
       <c r="C136">
         <v>0</v>
       </c>
       <c r="E136" t="s">
-        <v>245</v>
+        <v>148</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B137" t="s">
-        <v>381</v>
+        <v>443</v>
       </c>
       <c r="C137">
         <v>0</v>
       </c>
       <c r="E137" t="s">
-        <v>246</v>
+        <v>106</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B138" t="s">
-        <v>382</v>
+        <v>444</v>
       </c>
       <c r="C138">
         <v>0</v>
       </c>
       <c r="E138" t="s">
-        <v>240</v>
+        <v>103</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B139" t="s">
-        <v>462</v>
+        <v>445</v>
       </c>
       <c r="C139">
         <v>0</v>
       </c>
       <c r="E139" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B140" t="s">
-        <v>463</v>
+        <v>446</v>
       </c>
       <c r="C140">
         <v>0</v>
       </c>
       <c r="E140" t="s">
-        <v>109</v>
+        <v>249</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B141" t="s">
-        <v>464</v>
+        <v>447</v>
       </c>
       <c r="C141">
         <v>0</v>
       </c>
       <c r="E141" t="s">
-        <v>46</v>
+        <v>149</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B142" t="s">
-        <v>465</v>
+        <v>448</v>
       </c>
       <c r="C142">
         <v>0</v>
       </c>
       <c r="E142" t="s">
-        <v>156</v>
+        <v>106</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B143" t="s">
-        <v>466</v>
+        <v>449</v>
       </c>
       <c r="C143">
         <v>0</v>
       </c>
       <c r="E143" t="s">
-        <v>157</v>
+        <v>107</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B144" t="s">
-        <v>467</v>
+        <v>450</v>
       </c>
       <c r="C144">
         <v>0</v>
       </c>
       <c r="E144" t="s">
-        <v>115</v>
+        <v>150</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B145" t="s">
-        <v>468</v>
+        <v>361</v>
       </c>
       <c r="C145">
         <v>0</v>
       </c>
       <c r="E145" t="s">
-        <v>112</v>
+        <v>151</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B146" t="s">
-        <v>469</v>
+        <v>362</v>
       </c>
       <c r="C146">
         <v>0</v>
       </c>
       <c r="E146" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B147" t="s">
-        <v>470</v>
+        <v>363</v>
       </c>
       <c r="C147">
         <v>0</v>
       </c>
       <c r="E147" t="s">
-        <v>264</v>
+        <v>152</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B148" t="s">
-        <v>471</v>
+        <v>364</v>
       </c>
       <c r="C148">
         <v>0</v>
       </c>
       <c r="E148" t="s">
-        <v>158</v>
+        <v>100</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B149" t="s">
-        <v>472</v>
+        <v>365</v>
       </c>
       <c r="C149">
         <v>0</v>
       </c>
       <c r="E149" t="s">
-        <v>115</v>
+        <v>46</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B150" t="s">
-        <v>473</v>
+        <v>366</v>
       </c>
       <c r="C150">
         <v>0</v>
       </c>
       <c r="E150" t="s">
-        <v>116</v>
+        <v>153</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B151" t="s">
-        <v>474</v>
+        <v>367</v>
       </c>
       <c r="C151">
         <v>0</v>
       </c>
       <c r="E151" t="s">
-        <v>159</v>
+        <v>103</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B152" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="C152">
         <v>0</v>
       </c>
       <c r="E152" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B153" t="s">
-        <v>384</v>
+        <v>369</v>
       </c>
       <c r="C153">
         <v>0</v>
       </c>
       <c r="E153" t="s">
-        <v>17</v>
+        <v>155</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B154" t="s">
-        <v>385</v>
+        <v>370</v>
       </c>
       <c r="C154">
         <v>0</v>
       </c>
       <c r="E154" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B155" t="s">
-        <v>386</v>
+        <v>371</v>
       </c>
       <c r="C155">
         <v>0</v>
       </c>
       <c r="E155" t="s">
-        <v>109</v>
+        <v>157</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B156" t="s">
-        <v>387</v>
+        <v>372</v>
       </c>
       <c r="C156">
         <v>0</v>
       </c>
       <c r="E156" t="s">
-        <v>46</v>
+        <v>158</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B157" t="s">
-        <v>388</v>
+        <v>373</v>
       </c>
       <c r="C157">
         <v>0</v>
       </c>
       <c r="E157" t="s">
-        <v>162</v>
+        <v>247</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B158" t="s">
-        <v>389</v>
+        <v>374</v>
       </c>
       <c r="C158">
         <v>0</v>
       </c>
       <c r="E158" t="s">
-        <v>112</v>
+        <v>159</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B159" t="s">
-        <v>390</v>
+        <v>375</v>
       </c>
       <c r="C159">
         <v>0</v>
       </c>
       <c r="E159" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B160" t="s">
-        <v>391</v>
+        <v>376</v>
       </c>
       <c r="C160">
         <v>0</v>
       </c>
       <c r="E160" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B161" t="s">
-        <v>392</v>
+        <v>377</v>
       </c>
       <c r="C161">
         <v>0</v>
       </c>
       <c r="E161" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B162" t="s">
-        <v>393</v>
+        <v>378</v>
       </c>
       <c r="C162">
         <v>0</v>
       </c>
       <c r="E162" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B163" t="s">
-        <v>394</v>
+        <v>379</v>
       </c>
       <c r="C163">
         <v>0</v>
       </c>
       <c r="E163" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B164" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="C164">
         <v>0</v>
       </c>
       <c r="E164" t="s">
-        <v>262</v>
+        <v>165</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B165" t="s">
-        <v>396</v>
+        <v>381</v>
       </c>
       <c r="C165">
         <v>0</v>
       </c>
       <c r="E165" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B166" t="s">
-        <v>397</v>
+        <v>382</v>
       </c>
       <c r="C166">
         <v>0</v>
       </c>
       <c r="E166" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B167" t="s">
-        <v>398</v>
+        <v>383</v>
       </c>
       <c r="C167">
         <v>0</v>
       </c>
       <c r="E167" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B168" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
       <c r="C168">
         <v>0</v>
       </c>
       <c r="E168" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B169" t="s">
-        <v>400</v>
+        <v>385</v>
       </c>
       <c r="C169">
         <v>0</v>
       </c>
       <c r="E169" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B170" t="s">
-        <v>401</v>
+        <v>386</v>
       </c>
       <c r="C170">
         <v>0</v>
       </c>
       <c r="E170" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B171" t="s">
-        <v>402</v>
+        <v>387</v>
       </c>
       <c r="C171">
         <v>0</v>
       </c>
       <c r="E171" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B172" t="s">
-        <v>403</v>
+        <v>388</v>
       </c>
       <c r="C172">
         <v>0</v>
       </c>
       <c r="E172" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B173" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="C173">
         <v>0</v>
       </c>
       <c r="E173" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B174" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
       <c r="C174">
         <v>0</v>
       </c>
       <c r="E174" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B175" t="s">
-        <v>406</v>
+        <v>391</v>
       </c>
       <c r="C175">
         <v>0</v>
       </c>
       <c r="E175" t="s">
-        <v>178</v>
+        <v>142</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B176" t="s">
-        <v>407</v>
+        <v>392</v>
       </c>
       <c r="C176">
         <v>0</v>
       </c>
       <c r="E176" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>316</v>
+      </c>
+      <c r="B177" t="s">
+        <v>393</v>
+      </c>
+      <c r="C177">
+        <v>0</v>
+      </c>
+      <c r="E177" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>316</v>
+      </c>
+      <c r="B178" t="s">
+        <v>394</v>
+      </c>
+      <c r="C178">
+        <v>0</v>
+      </c>
+      <c r="E178" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>316</v>
+      </c>
+      <c r="B179" t="s">
+        <v>395</v>
+      </c>
+      <c r="C179">
+        <v>0</v>
+      </c>
+      <c r="E179" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>316</v>
+      </c>
+      <c r="B180" t="s">
+        <v>396</v>
+      </c>
+      <c r="C180">
+        <v>0</v>
+      </c>
+      <c r="E180" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>316</v>
+      </c>
+      <c r="B181" t="s">
+        <v>397</v>
+      </c>
+      <c r="C181">
+        <v>0</v>
+      </c>
+      <c r="E181" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>316</v>
+      </c>
+      <c r="B182" t="s">
+        <v>398</v>
+      </c>
+      <c r="C182">
+        <v>0</v>
+      </c>
+      <c r="E182" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A177" t="s">
-        <v>338</v>
-      </c>
-      <c r="B177" t="s">
-        <v>408</v>
-      </c>
-      <c r="C177">
-        <v>0</v>
-      </c>
-      <c r="E177" t="s">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>316</v>
+      </c>
+      <c r="B183" t="s">
+        <v>399</v>
+      </c>
+      <c r="C183">
+        <v>0</v>
+      </c>
+      <c r="E183" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A178" t="s">
-        <v>338</v>
-      </c>
-      <c r="B178" t="s">
-        <v>409</v>
-      </c>
-      <c r="C178">
-        <v>0</v>
-      </c>
-      <c r="E178" t="s">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>316</v>
+      </c>
+      <c r="B184" t="s">
+        <v>400</v>
+      </c>
+      <c r="C184">
+        <v>0</v>
+      </c>
+      <c r="E184" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A179" t="s">
-        <v>338</v>
-      </c>
-      <c r="B179" t="s">
-        <v>410</v>
-      </c>
-      <c r="C179">
-        <v>0</v>
-      </c>
-      <c r="E179" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A180" t="s">
-        <v>338</v>
-      </c>
-      <c r="B180" t="s">
-        <v>411</v>
-      </c>
-      <c r="C180">
-        <v>0</v>
-      </c>
-      <c r="E180" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A181" t="s">
-        <v>338</v>
-      </c>
-      <c r="B181" t="s">
-        <v>412</v>
-      </c>
-      <c r="C181">
-        <v>0</v>
-      </c>
-      <c r="E181" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A182" t="s">
-        <v>338</v>
-      </c>
-      <c r="B182" t="s">
-        <v>413</v>
-      </c>
-      <c r="C182">
-        <v>0</v>
-      </c>
-      <c r="E182" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A183" t="s">
-        <v>338</v>
-      </c>
-      <c r="B183" t="s">
-        <v>414</v>
-      </c>
-      <c r="C183">
-        <v>0</v>
-      </c>
-      <c r="E183" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A184" t="s">
-        <v>338</v>
-      </c>
-      <c r="B184" t="s">
-        <v>415</v>
-      </c>
-      <c r="C184">
-        <v>0</v>
-      </c>
-      <c r="E184" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B185" t="s">
-        <v>416</v>
+        <v>401</v>
       </c>
       <c r="C185">
         <v>0</v>
@@ -5138,82 +5051,94 @@
         <v>112</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="B186" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
       <c r="C186">
         <v>0</v>
       </c>
       <c r="E186" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>403</v>
+      </c>
+      <c r="B187" t="s">
+        <v>404</v>
+      </c>
+      <c r="C187">
+        <v>0</v>
+      </c>
+      <c r="E187" t="s">
+        <v>182</v>
+      </c>
+      <c r="F187" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>403</v>
+      </c>
+      <c r="B188" t="s">
+        <v>405</v>
+      </c>
+      <c r="C188">
+        <v>0</v>
+      </c>
+      <c r="E188" t="s">
+        <v>184</v>
+      </c>
+      <c r="F188" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>403</v>
+      </c>
+      <c r="B189" t="s">
+        <v>406</v>
+      </c>
+      <c r="C189">
+        <v>0</v>
+      </c>
+      <c r="E189" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A187" t="s">
-        <v>338</v>
-      </c>
-      <c r="B187" t="s">
-        <v>418</v>
-      </c>
-      <c r="C187">
-        <v>0</v>
-      </c>
-      <c r="E187" t="s">
+      <c r="F189" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A188" t="s">
-        <v>338</v>
-      </c>
-      <c r="B188" t="s">
-        <v>419</v>
-      </c>
-      <c r="C188">
-        <v>0</v>
-      </c>
-      <c r="E188" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A189" t="s">
-        <v>338</v>
-      </c>
-      <c r="B189" t="s">
-        <v>420</v>
-      </c>
-      <c r="C189">
-        <v>0</v>
-      </c>
-      <c r="E189" t="s">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>407</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C190">
+        <v>0</v>
+      </c>
+      <c r="E190" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A190" t="s">
-        <v>338</v>
-      </c>
-      <c r="B190" t="s">
-        <v>421</v>
-      </c>
-      <c r="C190">
-        <v>0</v>
-      </c>
-      <c r="E190" t="s">
+      <c r="F190" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>338</v>
-      </c>
-      <c r="B191" t="s">
-        <v>422</v>
+        <v>407</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>408</v>
       </c>
       <c r="C191">
         <v>0</v>
@@ -5221,583 +5146,439 @@
       <c r="E191" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F191" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>338</v>
+        <v>407</v>
       </c>
       <c r="B192" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
       <c r="C192">
         <v>0</v>
       </c>
       <c r="E192" t="s">
-        <v>121</v>
+        <v>192</v>
+      </c>
+      <c r="F192" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>338</v>
+        <v>407</v>
       </c>
       <c r="B193" t="s">
-        <v>424</v>
+        <v>410</v>
       </c>
       <c r="C193">
         <v>0</v>
       </c>
       <c r="E193" t="s">
-        <v>124</v>
+        <v>194</v>
+      </c>
+      <c r="F193" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>425</v>
+        <v>407</v>
       </c>
       <c r="B194" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
       <c r="C194">
         <v>0</v>
       </c>
       <c r="E194" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="F194" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>425</v>
+        <v>407</v>
       </c>
       <c r="B195" t="s">
-        <v>427</v>
+        <v>412</v>
       </c>
       <c r="C195">
         <v>0</v>
       </c>
       <c r="E195" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="F195" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>425</v>
-      </c>
-      <c r="B196" t="s">
-        <v>428</v>
-      </c>
-      <c r="C196">
-        <v>0</v>
-      </c>
-      <c r="E196" t="s">
-        <v>195</v>
+        <v>413</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="C196" s="2">
+        <v>0</v>
+      </c>
+      <c r="D196" s="2"/>
+      <c r="E196" s="2" t="s">
+        <v>200</v>
       </c>
       <c r="F196" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>429</v>
-      </c>
-      <c r="B197" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="C197">
-        <v>0</v>
-      </c>
-      <c r="E197" t="s">
-        <v>197</v>
+        <v>413</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="C197" s="2">
+        <v>0</v>
+      </c>
+      <c r="D197" s="2"/>
+      <c r="E197" s="2" t="s">
+        <v>202</v>
       </c>
       <c r="F197" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>429</v>
-      </c>
-      <c r="B198" s="3" t="s">
-        <v>430</v>
+        <v>413</v>
+      </c>
+      <c r="B198" t="s">
+        <v>416</v>
       </c>
       <c r="C198">
         <v>0</v>
       </c>
       <c r="E198" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="F198" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>429</v>
-      </c>
-      <c r="B199" t="s">
-        <v>431</v>
-      </c>
-      <c r="C199">
-        <v>0</v>
-      </c>
-      <c r="E199" t="s">
-        <v>201</v>
+        <v>413</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C199" s="3">
+        <v>0</v>
+      </c>
+      <c r="D199" s="3"/>
+      <c r="E199" s="3" t="s">
+        <v>205</v>
       </c>
       <c r="F199" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>429</v>
-      </c>
-      <c r="B200" t="s">
-        <v>432</v>
-      </c>
-      <c r="C200">
-        <v>0</v>
-      </c>
-      <c r="E200" t="s">
-        <v>231</v>
+        <v>413</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="C200" s="3">
+        <v>0</v>
+      </c>
+      <c r="D200" s="3"/>
+      <c r="E200" s="3" t="s">
+        <v>207</v>
       </c>
       <c r="F200" t="s">
-        <v>233</v>
+        <v>208</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="B201" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="C201">
         <v>0</v>
       </c>
       <c r="E201" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="F201" t="s">
-        <v>232</v>
+        <v>210</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="B202" t="s">
-        <v>434</v>
+        <v>419</v>
       </c>
       <c r="C202">
         <v>0</v>
       </c>
       <c r="E202" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="F202" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>429</v>
-      </c>
-      <c r="B203" t="s">
-        <v>435</v>
+        <v>413</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>420</v>
       </c>
       <c r="C203">
         <v>0</v>
       </c>
       <c r="E203" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="F203" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>429</v>
-      </c>
-      <c r="B204" t="s">
-        <v>436</v>
-      </c>
-      <c r="C204">
-        <v>0</v>
-      </c>
-      <c r="E204" t="s">
-        <v>207</v>
+        <v>413</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="C204" s="3">
+        <v>0</v>
+      </c>
+      <c r="D204" s="3"/>
+      <c r="E204" s="3" t="s">
+        <v>209</v>
       </c>
       <c r="F204" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>437</v>
-      </c>
-      <c r="B205" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="C205" s="2">
-        <v>0</v>
-      </c>
-      <c r="D205" s="2"/>
-      <c r="E205" s="2" t="s">
-        <v>209</v>
+        <v>413</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C205" s="3">
+        <v>0</v>
+      </c>
+      <c r="D205" s="3"/>
+      <c r="E205" s="3" t="s">
+        <v>215</v>
       </c>
       <c r="F205" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>437</v>
-      </c>
-      <c r="B206" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="C206" s="2">
-        <v>0</v>
-      </c>
-      <c r="D206" s="2"/>
-      <c r="E206" s="2" t="s">
-        <v>211</v>
+        <v>413</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="C206">
+        <v>0</v>
+      </c>
+      <c r="E206" t="s">
+        <v>217</v>
       </c>
       <c r="F206" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>437</v>
-      </c>
-      <c r="B207" t="s">
-        <v>440</v>
+        <v>413</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>424</v>
       </c>
       <c r="C207">
         <v>0</v>
       </c>
       <c r="E207" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="F207" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
+        <v>316</v>
+      </c>
+      <c r="B208" t="s">
+        <v>425</v>
+      </c>
+      <c r="C208">
+        <v>0</v>
+      </c>
+      <c r="E208" t="s">
+        <v>248</v>
+      </c>
+      <c r="F208" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>316</v>
+      </c>
+      <c r="B209" t="s">
+        <v>426</v>
+      </c>
+      <c r="C209">
+        <v>0</v>
+      </c>
+      <c r="E209" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>316</v>
+      </c>
+      <c r="B210" t="s">
+        <v>427</v>
+      </c>
+      <c r="C210">
+        <v>0</v>
+      </c>
+      <c r="E210" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>316</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C211" s="2">
+        <v>0</v>
+      </c>
+      <c r="D211" s="2"/>
+      <c r="E211" s="2" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>316</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C212" s="2">
+        <v>0</v>
+      </c>
+      <c r="D212" s="2"/>
+      <c r="E212" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>316</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="C213" s="2">
+        <v>0</v>
+      </c>
+      <c r="D213" s="2"/>
+      <c r="E213" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>316</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="C214" s="2">
+        <v>0</v>
+      </c>
+      <c r="D214" s="2"/>
+      <c r="E214" s="2" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>316</v>
+      </c>
+      <c r="B215" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="B208" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="C208" s="3">
-        <v>0</v>
-      </c>
-      <c r="D208" s="3"/>
-      <c r="E208" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="F208" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A209" t="s">
-        <v>437</v>
-      </c>
-      <c r="B209" s="3" t="s">
-        <v>441</v>
-      </c>
-      <c r="C209" s="3">
-        <v>0</v>
-      </c>
-      <c r="D209" s="3"/>
-      <c r="E209" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="F209" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A210" t="s">
-        <v>437</v>
-      </c>
-      <c r="B210" t="s">
-        <v>442</v>
-      </c>
-      <c r="C210">
-        <v>0</v>
-      </c>
-      <c r="E210" t="s">
-        <v>218</v>
-      </c>
-      <c r="F210" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A211" t="s">
-        <v>437</v>
-      </c>
-      <c r="B211" t="s">
-        <v>443</v>
-      </c>
-      <c r="C211">
-        <v>0</v>
-      </c>
-      <c r="E211" t="s">
-        <v>220</v>
-      </c>
-      <c r="F211" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A212" t="s">
-        <v>437</v>
-      </c>
-      <c r="B212" s="3" t="s">
-        <v>444</v>
-      </c>
-      <c r="C212">
-        <v>0</v>
-      </c>
-      <c r="E212" t="s">
-        <v>222</v>
-      </c>
-      <c r="F212" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A213" t="s">
-        <v>437</v>
-      </c>
-      <c r="B213" s="3" t="s">
-        <v>445</v>
-      </c>
-      <c r="C213" s="3">
-        <v>0</v>
-      </c>
-      <c r="D213" s="3"/>
-      <c r="E213" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="F213" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A214" t="s">
-        <v>437</v>
-      </c>
-      <c r="B214" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="C214" s="3">
-        <v>0</v>
-      </c>
-      <c r="D214" s="3"/>
-      <c r="E214" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="F214" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A215" t="s">
-        <v>437</v>
-      </c>
-      <c r="B215" s="3" t="s">
-        <v>447</v>
-      </c>
-      <c r="C215">
-        <v>0</v>
-      </c>
-      <c r="E215" t="s">
-        <v>226</v>
-      </c>
-      <c r="F215" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C215" s="2">
+        <v>0</v>
+      </c>
+      <c r="D215" s="2"/>
+      <c r="E215" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>437</v>
-      </c>
-      <c r="B216" s="3" t="s">
-        <v>448</v>
-      </c>
-      <c r="C216">
-        <v>0</v>
-      </c>
-      <c r="E216" t="s">
-        <v>228</v>
-      </c>
-      <c r="F216" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
+        <v>316</v>
+      </c>
+      <c r="B216" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="C216" s="6">
+        <v>0</v>
+      </c>
+      <c r="E216" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>338</v>
-      </c>
-      <c r="B217" t="s">
-        <v>449</v>
-      </c>
-      <c r="C217">
-        <v>0</v>
-      </c>
-      <c r="E217" t="s">
-        <v>263</v>
-      </c>
-      <c r="F217" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A218" t="s">
-        <v>338</v>
-      </c>
-      <c r="B218" t="s">
-        <v>450</v>
-      </c>
-      <c r="C218">
-        <v>0</v>
-      </c>
-      <c r="E218" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A219" t="s">
-        <v>338</v>
-      </c>
-      <c r="B219" t="s">
-        <v>451</v>
-      </c>
-      <c r="C219">
-        <v>0</v>
-      </c>
-      <c r="E219" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A220" t="s">
-        <v>338</v>
-      </c>
-      <c r="B220" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="C220" s="2">
-        <v>0</v>
-      </c>
-      <c r="D220" s="2"/>
-      <c r="E220" s="2" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A221" t="s">
-        <v>338</v>
-      </c>
-      <c r="B221" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="C221" s="2">
-        <v>0</v>
-      </c>
-      <c r="D221" s="2"/>
-      <c r="E221" s="2" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A222" t="s">
-        <v>338</v>
-      </c>
-      <c r="B222" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="C222" s="2">
-        <v>0</v>
-      </c>
-      <c r="D222" s="2"/>
-      <c r="E222" s="2" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A223" t="s">
-        <v>338</v>
-      </c>
-      <c r="B223" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="C223" s="2">
-        <v>0</v>
-      </c>
-      <c r="D223" s="2"/>
-      <c r="E223" s="2" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A224" t="s">
-        <v>338</v>
-      </c>
-      <c r="B224" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="C224" s="2">
-        <v>0</v>
-      </c>
-      <c r="D224" s="2"/>
-      <c r="E224" s="2" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A225" t="s">
-        <v>338</v>
-      </c>
-      <c r="B225" s="6" t="s">
-        <v>507</v>
-      </c>
-      <c r="C225" s="6">
-        <v>0</v>
-      </c>
-      <c r="E225" s="6" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A226" t="s">
-        <v>338</v>
-      </c>
-      <c r="B226" s="6" t="s">
-        <v>509</v>
-      </c>
-      <c r="C226" s="6">
-        <v>0</v>
-      </c>
-      <c r="E226" s="6" t="s">
-        <v>510</v>
+        <v>316</v>
+      </c>
+      <c r="B217" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="C217" s="6">
+        <v>0</v>
+      </c>
+      <c r="E217" s="6" t="s">
+        <v>486</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <autoFilter ref="A1:F224"/>
+  <autoFilter ref="A1:F215"/>
   <sortState ref="A2:B224">
     <sortCondition ref="B2"/>
   </sortState>

</xml_diff>

<commit_message>
use company schema by default
</commit_message>
<xml_diff>
--- a/database/seeds/data/fragments.xlsx
+++ b/database/seeds/data/fragments.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27715"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/willem/Sites/blender/database/seeds/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/freek/dev/sites/blender/database/seeds/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28260"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="27200"/>
   </bookViews>
   <sheets>
     <sheet name="fragments" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="490">
   <si>
     <t>name</t>
   </si>
@@ -1492,13 +1492,22 @@
   </si>
   <si>
     <t>Publieke site</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>googleMyBusinessUrl</t>
+  </si>
+  <si>
+    <t>fax</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1508,6 +1517,12 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -1535,10 +1550,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1548,8 +1564,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1856,7 +1875,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
+      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2313,7 +2332,122 @@
         <v>246</v>
       </c>
     </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="7"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="8"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="7"/>
       <c r="F36" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bring some fragments back
</commit_message>
<xml_diff>
--- a/database/seeds/data/fragments.xlsx
+++ b/database/seeds/data/fragments.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="166">
   <si>
     <t>name</t>
   </si>
@@ -138,12 +138,156 @@
     <t>Adres</t>
   </si>
   <si>
+    <t>Wijzig wachtwoord</t>
+  </si>
+  <si>
+    <t>Changer mot de passe</t>
+  </si>
+  <si>
+    <t>Stad</t>
+  </si>
+  <si>
+    <t>Land</t>
+  </si>
+  <si>
+    <t>De inloggegevens klopten niet.</t>
+  </si>
+  <si>
+    <t>Wachtwoord vergeten?</t>
+  </si>
+  <si>
+    <t>Mot de passe oublié?</t>
+  </si>
+  <si>
+    <t>Deze link is ongeldig.</t>
+  </si>
+  <si>
+    <t>Ce lien n'est pas valable.</t>
+  </si>
+  <si>
     <t>Naam</t>
   </si>
   <si>
+    <t>Je bent nu uitgelogd.</t>
+  </si>
+  <si>
+    <t>Vous êtes déconnecté(e).</t>
+  </si>
+  <si>
+    <t>Log in</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>Nog geen account?</t>
+  </si>
+  <si>
+    <t>Les données ne sont pas correctes.</t>
+  </si>
+  <si>
+    <t>Uw account is nog niet actief.</t>
+  </si>
+  <si>
+    <t>Votre compte n'est pas encore actif.</t>
+  </si>
+  <si>
+    <t>Uw wachtwoord werd gewijzigd.</t>
+  </si>
+  <si>
+    <t>Votre mot de passe a été changé.</t>
+  </si>
+  <si>
+    <t>Wachtwoord instellen</t>
+  </si>
+  <si>
     <t>Postcode</t>
   </si>
   <si>
+    <t>Registreer</t>
+  </si>
+  <si>
+    <t>Maak profiel aan</t>
+  </si>
+  <si>
+    <t>Créez votre profil</t>
+  </si>
+  <si>
+    <t>Naar login</t>
+  </si>
+  <si>
+    <t>Vers login</t>
+  </si>
+  <si>
+    <t>Je nieuwe wachtwoord moet minstens 8 karakters lang zijn.</t>
+  </si>
+  <si>
+    <t>Votre nouveau mot de passe doit contenir au moins 8 caractères.</t>
+  </si>
+  <si>
+    <t>Deze link is niet meer geldig.</t>
+  </si>
+  <si>
+    <t>Ce lien n'est plus valable.</t>
+  </si>
+  <si>
+    <t>Mail me</t>
+  </si>
+  <si>
+    <t>Envoyez-moi l'e-mail</t>
+  </si>
+  <si>
+    <t>Geef je e-mailadres op en we sturen je een link waarmee je je wachtwoord kan wijzigen</t>
+  </si>
+  <si>
+    <t>Donnez-nous votre adresse e-mail et nous vous envoyons un lien par lequel vous pouvez changer votre mot de passe</t>
+  </si>
+  <si>
+    <t>Wachtwoord opvragen</t>
+  </si>
+  <si>
+    <t>Demander mot de passe</t>
+  </si>
+  <si>
+    <t>Geef je e-mailadres op en we sturen je een link waarmee je je wachtwoord kan wijzigen.</t>
+  </si>
+  <si>
+    <t>Donnez votre adresse e-mail et nous vous envoyons un lien par lequel vous pouvez changer votre mot de passe.</t>
+  </si>
+  <si>
+    <t>Initialiser mot de passe</t>
+  </si>
+  <si>
+    <t>Inloggen?</t>
+  </si>
+  <si>
+    <t>Connecter?</t>
+  </si>
+  <si>
+    <t>Nog geen profiel?</t>
+  </si>
+  <si>
+    <t>Pas encore de profil?</t>
+  </si>
+  <si>
+    <t>Er is niemand geregistreerd met dit e-mailadres.</t>
+  </si>
+  <si>
+    <t>Cette adresse e-mail n'est pas connue.</t>
+  </si>
+  <si>
+    <t>Uw aanvraag is ontvangen. Er worden er bevestiging gestuurd zodra deze wordt goedgekeurd.</t>
+  </si>
+  <si>
+    <t>Nous avons reçu votre demande. Vous recevrez une confirmation dès qu'elle sera approuvée.</t>
+  </si>
+  <si>
+    <t>Uitloggen</t>
+  </si>
+  <si>
     <t>Voor deze sites gebruiken we cookies om de gebruikservaring te verbeteren. Indien u verder surft gaan we ervan uit dat u cookies toelaat.</t>
   </si>
   <si>
@@ -279,7 +423,103 @@
     <t>fieldsAreRequired</t>
   </si>
   <si>
+    <t>auth</t>
+  </si>
+  <si>
+    <t>changePassword</t>
+  </si>
+  <si>
     <t>country</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>forgotPassword</t>
+  </si>
+  <si>
+    <t>invalidResetLink</t>
+  </si>
+  <si>
+    <t>loggedOut</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>logout</t>
+  </si>
+  <si>
+    <t>logout.title</t>
+  </si>
+  <si>
+    <t>noAccount</t>
+  </si>
+  <si>
+    <t>notActivatedError</t>
+  </si>
+  <si>
+    <t>passwordChanged</t>
+  </si>
+  <si>
+    <t>passwordConfirm</t>
+  </si>
+  <si>
+    <t>register</t>
+  </si>
+  <si>
+    <t>register.submit</t>
+  </si>
+  <si>
+    <t>register.toLogin</t>
+  </si>
+  <si>
+    <t>resetInstructions</t>
+  </si>
+  <si>
+    <t>resetLinkExpired</t>
+  </si>
+  <si>
+    <t>resetPassword.button</t>
+  </si>
+  <si>
+    <t>resetPassword.intro</t>
+  </si>
+  <si>
+    <t>resetPassword.title</t>
+  </si>
+  <si>
+    <t>resetPassword.toLogin</t>
+  </si>
+  <si>
+    <t>resetPasswordButton</t>
+  </si>
+  <si>
+    <t>resetPasswordIntro</t>
+  </si>
+  <si>
+    <t>titleChangePassword</t>
+  </si>
+  <si>
+    <t>titleLogin</t>
+  </si>
+  <si>
+    <t>titleRegister</t>
+  </si>
+  <si>
+    <t>titleResetPassword</t>
+  </si>
+  <si>
+    <t>toLogin</t>
+  </si>
+  <si>
+    <t>toRegistrationForm</t>
+  </si>
+  <si>
+    <t>unknownUser</t>
+  </si>
+  <si>
+    <t>waitingForApproval</t>
   </si>
   <si>
     <t>company</t>
@@ -678,10 +918,10 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -719,10 +959,10 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>108</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -736,10 +976,10 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>109</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -753,10 +993,10 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -770,10 +1010,10 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>111</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -787,10 +1027,10 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>107</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>112</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -804,10 +1044,10 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>107</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -821,10 +1061,10 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>114</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -838,10 +1078,10 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>115</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -855,10 +1095,10 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>116</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -872,10 +1112,10 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>117</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -889,10 +1129,10 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>118</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -906,10 +1146,10 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>119</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -923,10 +1163,10 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>120</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -940,10 +1180,10 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -957,10 +1197,10 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -974,155 +1214,155 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>122</v>
       </c>
       <c r="E17" t="s">
-        <v>37</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="E18" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="F19" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="E20" t="s">
         <v>30</v>
       </c>
       <c r="F20" t="s">
-        <v>44</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>114</v>
       </c>
       <c r="E21" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="F21" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>124</v>
       </c>
       <c r="E22" t="s">
         <v>34</v>
       </c>
       <c r="F22" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>125</v>
       </c>
       <c r="E23" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="F23" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>126</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="F24" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>104</v>
       </c>
       <c r="B25" t="s">
-        <v>79</v>
+        <v>127</v>
       </c>
       <c r="E25" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
       <c r="F25" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>104</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>128</v>
       </c>
       <c r="E26" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="F26" t="s">
-        <v>50</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
       <c r="E27" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="F27" t="s">
-        <v>51</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>83</v>
+        <v>163</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>0</v>
@@ -1135,10 +1375,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>83</v>
+        <v>163</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>76</v>
+        <v>124</v>
       </c>
       <c r="C29" s="2">
         <v>0</v>
@@ -1148,10 +1388,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>83</v>
+        <v>163</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>84</v>
+        <v>164</v>
       </c>
       <c r="C30" s="2">
         <v>0</v>
@@ -1161,10 +1401,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>83</v>
+        <v>163</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>77</v>
+        <v>125</v>
       </c>
       <c r="C31" s="2">
         <v>0</v>
@@ -1174,10 +1414,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>83</v>
+        <v>163</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>78</v>
+        <v>126</v>
       </c>
       <c r="C32" s="2">
         <v>0</v>
@@ -1187,10 +1427,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>83</v>
+        <v>163</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>82</v>
+        <v>132</v>
       </c>
       <c r="C33" s="2">
         <v>0</v>
@@ -1200,10 +1440,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>83</v>
+        <v>163</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="C34" s="2">
         <v>0</v>
@@ -1213,10 +1453,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>83</v>
+        <v>163</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>85</v>
+        <v>165</v>
       </c>
       <c r="C35" s="2">
         <v>0</v>
@@ -1226,10 +1466,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>83</v>
+        <v>163</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>66</v>
+        <v>114</v>
       </c>
       <c r="C36" s="2">
         <v>0</v>
@@ -1253,8 +1493,8 @@
   <dimension ref="A1:AA217"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F178" sqref="F178"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E159" sqref="E159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1269,10 +1509,10 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1308,6 +1548,653 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" t="s">
+        <v>142</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" t="s">
+        <v>143</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22" t="s">
+        <v>144</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" t="s">
+        <v>145</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24" t="s">
+        <v>146</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>130</v>
+      </c>
+      <c r="B25" t="s">
+        <v>147</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>130</v>
+      </c>
+      <c r="B26" t="s">
+        <v>148</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>130</v>
+      </c>
+      <c r="B27" t="s">
+        <v>149</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>130</v>
+      </c>
+      <c r="B28" t="s">
+        <v>150</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>130</v>
+      </c>
+      <c r="B29" t="s">
+        <v>151</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>71</v>
+      </c>
+      <c r="F29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>130</v>
+      </c>
+      <c r="B30" t="s">
+        <v>152</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>130</v>
+      </c>
+      <c r="B31" t="s">
+        <v>153</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>67</v>
+      </c>
+      <c r="F31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" t="s">
+        <v>154</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="E32" t="s">
+        <v>73</v>
+      </c>
+      <c r="F32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>130</v>
+      </c>
+      <c r="B33" t="s">
+        <v>121</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" t="s">
+        <v>155</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" t="s">
+        <v>156</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36" t="s">
+        <v>157</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>59</v>
+      </c>
+      <c r="F36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>130</v>
+      </c>
+      <c r="B37" t="s">
+        <v>158</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>130</v>
+      </c>
+      <c r="B38" t="s">
+        <v>159</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
+        <v>76</v>
+      </c>
+      <c r="F38" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>130</v>
+      </c>
+      <c r="B39" t="s">
+        <v>160</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
+        <v>78</v>
+      </c>
+      <c r="F39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>130</v>
+      </c>
+      <c r="B40" t="s">
+        <v>161</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>80</v>
+      </c>
+      <c r="F40" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>130</v>
+      </c>
+      <c r="B41" t="s">
+        <v>162</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>82</v>
+      </c>
+      <c r="F41" t="s">
+        <v>83</v>
+      </c>
+    </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>

</xml_diff>